<commit_message>
Added package installation code
</commit_message>
<xml_diff>
--- a/Data/polls.xlsx
+++ b/Data/polls.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mac Tan\Desktop\Mac's Stuff\Elections\2019\Israel-2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mac Tan\Desktop\Mac's Stuff\Elections\2019\Israel-2019\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0E67CF-2027-465B-A51C-D0D7A5F72887}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEC8E90-CD13-405B-AEF4-C06B6230CB09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="3" xr2:uid="{0DE1B94D-B05B-4FF7-9BF3-1803C0C1CFBD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="251">
   <si>
     <t>Channel 2[5]</t>
   </si>
@@ -782,6 +782,12 @@
   </si>
   <si>
     <t>Maagar Mochot/Radio 103 FM[4]</t>
+  </si>
+  <si>
+    <t>Maagar Mochot/Israel Hayom &amp; i24 News[4]</t>
+  </si>
+  <si>
+    <t>Midgam/iPanel/Yediot Ahronot[5]</t>
   </si>
 </sst>
 </file>
@@ -8959,10 +8965,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CC49F9-512D-4648-8DF6-8D5ABA179EFE}">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -9037,67 +9043,67 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>43518</v>
+        <v>43520</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V2">
         <f>SUM(C2:P2)</f>
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>43517</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>242</v>
+        <v>43520</v>
+      </c>
+      <c r="B3" t="s">
+        <v>250</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -9106,7 +9112,7 @@
         <v>4</v>
       </c>
       <c r="F3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>35</v>
@@ -9127,10 +9133,10 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O3">
         <v>5</v>
@@ -9145,25 +9151,25 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>43517</v>
+        <v>43518</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G4">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H4">
         <v>4</v>
@@ -9175,7 +9181,7 @@
         <v>4</v>
       </c>
       <c r="K4">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -9184,31 +9190,31 @@
         <v>6</v>
       </c>
       <c r="N4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P4">
         <v>6</v>
       </c>
       <c r="V4">
-        <f>SUM(C4:P4)</f>
-        <v>120</v>
+        <f t="shared" ref="V2:V10" si="0">SUM(C4:P4)</f>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>43517</v>
       </c>
-      <c r="B5" t="s">
-        <v>244</v>
+      <c r="B5" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -9220,16 +9226,16 @@
         <v>35</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K5">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -9247,7 +9253,7 @@
         <v>7</v>
       </c>
       <c r="V5">
-        <f>SUM(C5:P5)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
@@ -9256,13 +9262,13 @@
         <v>43517</v>
       </c>
       <c r="B6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -9271,37 +9277,37 @@
         <v>8</v>
       </c>
       <c r="G6">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K6">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P6">
         <v>6</v>
       </c>
       <c r="V6">
-        <f>SUM(C6:P6)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
@@ -9310,43 +9316,43 @@
         <v>43517</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O7">
         <v>5</v>
@@ -9355,7 +9361,7 @@
         <v>7</v>
       </c>
       <c r="V7">
-        <f>SUM(C7:P7)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
@@ -9364,25 +9370,25 @@
         <v>43517</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -9391,106 +9397,94 @@
         <v>5</v>
       </c>
       <c r="K8">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O8">
         <v>6</v>
       </c>
       <c r="P8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V8">
-        <f>SUM(C8:P8)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="B9" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9">
-        <f>R9+T9</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H9">
         <v>4</v>
       </c>
       <c r="I9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K9">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P9">
         <v>7</v>
       </c>
-      <c r="Q9">
-        <v>5</v>
-      </c>
-      <c r="R9">
-        <v>13</v>
-      </c>
-      <c r="S9">
-        <v>5</v>
-      </c>
-      <c r="T9">
-        <v>19</v>
-      </c>
-      <c r="U9">
-        <v>6</v>
+      <c r="V9">
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>43513</v>
+        <v>43517</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -9499,8 +9493,7 @@
         <v>5</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:G35" si="0">R10+T10</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H10">
         <v>4</v>
@@ -9509,51 +9502,40 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K10">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N10">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P10">
-        <v>6</v>
-      </c>
-      <c r="Q10">
-        <v>7</v>
-      </c>
-      <c r="R10">
-        <v>10</v>
-      </c>
-      <c r="S10">
-        <v>5</v>
-      </c>
-      <c r="T10">
-        <v>24</v>
-      </c>
-      <c r="U10">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>43513</v>
+        <v>43516</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -9562,35 +9544,35 @@
         <v>5</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f>R11+T11</f>
+        <v>32</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
         <v>0</v>
       </c>
-      <c r="J11">
-        <v>4</v>
-      </c>
       <c r="K11">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P11">
         <v>7</v>
@@ -9599,40 +9581,40 @@
         <v>5</v>
       </c>
       <c r="R11">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T11">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U11">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>43512</v>
+        <v>43513</v>
       </c>
       <c r="B12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f t="shared" ref="G12:G37" si="1">R12+T12</f>
+        <v>34</v>
       </c>
       <c r="H12">
         <v>4</v>
@@ -9641,28 +9623,28 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K12">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N12">
         <v>5</v>
       </c>
       <c r="O12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P12">
         <v>6</v>
       </c>
       <c r="Q12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R12">
         <v>10</v>
@@ -9671,7 +9653,7 @@
         <v>5</v>
       </c>
       <c r="T12">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="U12">
         <v>6</v>
@@ -9679,35 +9661,35 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>43509</v>
+        <v>43513</v>
       </c>
       <c r="B13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="H13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K13">
         <v>30</v>
@@ -9716,64 +9698,64 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P13">
         <v>7</v>
       </c>
       <c r="Q13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T13">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="U13">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>43508</v>
+        <v>43512</v>
       </c>
       <c r="B14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>5</v>
       </c>
       <c r="F14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="H14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K14">
         <v>30</v>
@@ -9782,79 +9764,79 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R14">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T14">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U14">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>43508</v>
+        <v>43509</v>
       </c>
       <c r="B15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>6</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="H15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K15">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P15">
         <v>7</v>
@@ -9869,18 +9851,18 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U15">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>43504</v>
+        <v>43508</v>
       </c>
       <c r="B16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C16">
         <v>7</v>
@@ -9892,32 +9874,32 @@
         <v>5</v>
       </c>
       <c r="F16">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
-        <v>34</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K16">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O16">
         <v>6</v>
@@ -9932,10 +9914,10 @@
         <v>11</v>
       </c>
       <c r="S16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="U16">
         <v>7</v>
@@ -9943,26 +9925,26 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>43503</v>
+        <v>43508</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="C17">
         <v>7</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <v>5</v>
       </c>
       <c r="F17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="H17">
         <v>5</v>
@@ -9971,7 +9953,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K17">
         <v>32</v>
@@ -9992,7 +9974,7 @@
         <v>7</v>
       </c>
       <c r="Q17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R17">
         <v>11</v>
@@ -10001,7 +9983,7 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U17">
         <v>7</v>
@@ -10009,35 +9991,35 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>43503</v>
+        <v>43504</v>
       </c>
       <c r="B18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="H18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K18">
         <v>32</v>
@@ -10046,31 +10028,31 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q18">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R18">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T18">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U18">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -10078,23 +10060,23 @@
         <v>43503</v>
       </c>
       <c r="B19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E19">
         <v>5</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="H19">
         <v>5</v>
@@ -10103,40 +10085,40 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K19">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P19">
         <v>7</v>
       </c>
       <c r="Q19">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R19">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T19">
         <v>22</v>
       </c>
       <c r="U19">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -10144,125 +10126,125 @@
         <v>43503</v>
       </c>
       <c r="B20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
         <v>0</v>
       </c>
-      <c r="D20">
-        <v>11</v>
-      </c>
-      <c r="E20">
-        <v>7</v>
-      </c>
-      <c r="F20">
-        <v>5</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>5</v>
-      </c>
       <c r="J20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K20">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P20">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q20">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="R20">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T20">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="U20">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>43502</v>
+        <v>43503</v>
       </c>
       <c r="B21" t="s">
-        <v>221</v>
+        <v>154</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21">
         <v>5</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
         <v>34</v>
-      </c>
-      <c r="H21">
-        <v>5</v>
-      </c>
-      <c r="I21">
-        <v>4</v>
-      </c>
-      <c r="J21">
-        <v>5</v>
-      </c>
-      <c r="K21">
-        <v>30</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R21">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T21">
         <v>22</v>
@@ -10273,38 +10255,38 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>43502</v>
+        <v>43503</v>
       </c>
       <c r="B22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="H22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
         <v>0</v>
       </c>
-      <c r="J22">
-        <v>5</v>
-      </c>
       <c r="K22">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -10313,52 +10295,52 @@
         <v>7</v>
       </c>
       <c r="N22">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P22">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q22">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="R22">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="S22">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T22">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U22">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>43500</v>
+        <v>43502</v>
       </c>
       <c r="B23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F23">
         <v>5</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
       <c r="H23">
         <v>5</v>
@@ -10376,10 +10358,10 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O23">
         <v>5</v>
@@ -10388,187 +10370,187 @@
         <v>6</v>
       </c>
       <c r="Q23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R23">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T23">
         <v>22</v>
       </c>
       <c r="U23">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>43497</v>
+        <v>43502</v>
       </c>
       <c r="B24" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24">
         <v>6</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24">
         <v>32</v>
-      </c>
-      <c r="H24">
-        <v>5</v>
-      </c>
-      <c r="I24">
-        <v>4</v>
-      </c>
-      <c r="J24">
-        <v>5</v>
-      </c>
-      <c r="K24">
-        <v>31</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R24">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T24">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="U24">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>43496</v>
+        <v>43500</v>
       </c>
       <c r="B25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>30</v>
+      </c>
+      <c r="L25">
         <v>0</v>
       </c>
-      <c r="D25">
-        <v>9</v>
-      </c>
-      <c r="E25">
-        <v>4</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="H25">
-        <v>5</v>
-      </c>
-      <c r="I25">
-        <v>4</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>28</v>
-      </c>
-      <c r="L25">
-        <v>4</v>
-      </c>
       <c r="M25">
         <v>7</v>
       </c>
       <c r="N25">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R25">
         <v>9</v>
       </c>
       <c r="S25">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T25">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="U25">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>43495</v>
+        <v>43497</v>
       </c>
       <c r="B26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F26">
         <v>6</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="H26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I26">
         <v>4</v>
       </c>
       <c r="J26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K26">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -10580,49 +10562,49 @@
         <v>4</v>
       </c>
       <c r="O26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R26">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S26">
         <v>4</v>
       </c>
       <c r="T26">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="U26">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>43495</v>
+        <v>43496</v>
       </c>
       <c r="B27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C27">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E27">
         <v>4</v>
       </c>
       <c r="F27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
       <c r="H27">
         <v>5</v>
@@ -10631,40 +10613,40 @@
         <v>4</v>
       </c>
       <c r="J27">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K27">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="M27">
+        <v>7</v>
+      </c>
+      <c r="N27">
         <v>0</v>
       </c>
-      <c r="M27">
-        <v>7</v>
-      </c>
-      <c r="N27">
-        <v>4</v>
-      </c>
       <c r="O27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P27">
         <v>7</v>
       </c>
       <c r="Q27">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R27">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S27">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T27">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U27">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -10672,47 +10654,47 @@
         <v>43495</v>
       </c>
       <c r="B28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D28">
         <v>6</v>
       </c>
       <c r="E28">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F28">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="H28">
         <v>4</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K28">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N28">
         <v>4</v>
       </c>
       <c r="O28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P28">
         <v>6</v>
@@ -10727,10 +10709,10 @@
         <v>4</v>
       </c>
       <c r="T28">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U28">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -10738,23 +10720,23 @@
         <v>43495</v>
       </c>
       <c r="B29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="H29">
         <v>5</v>
@@ -10763,10 +10745,10 @@
         <v>4</v>
       </c>
       <c r="J29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K29">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -10778,33 +10760,33 @@
         <v>4</v>
       </c>
       <c r="O29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P29">
         <v>7</v>
       </c>
       <c r="Q29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R29">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S29">
         <v>4</v>
       </c>
       <c r="T29">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="U29">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>43489</v>
+        <v>43495</v>
       </c>
       <c r="B30" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C30">
         <v>6</v>
@@ -10816,17 +10798,17 @@
         <v>6</v>
       </c>
       <c r="F30">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="H30">
         <v>4</v>
       </c>
       <c r="I30">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J30">
         <v>5</v>
@@ -10844,7 +10826,7 @@
         <v>4</v>
       </c>
       <c r="O30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P30">
         <v>6</v>
@@ -10853,13 +10835,13 @@
         <v>6</v>
       </c>
       <c r="R30">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S30">
         <v>4</v>
       </c>
       <c r="T30">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="U30">
         <v>6</v>
@@ -10867,32 +10849,32 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>43487</v>
+        <v>43495</v>
       </c>
       <c r="B31" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E31">
         <v>5</v>
       </c>
       <c r="F31">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="H31">
         <v>5</v>
       </c>
       <c r="I31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J31">
         <v>5</v>
@@ -10910,64 +10892,67 @@
         <v>4</v>
       </c>
       <c r="O31">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P31">
         <v>7</v>
       </c>
       <c r="Q31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R31">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S31">
         <v>4</v>
       </c>
       <c r="T31">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="U31">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>43482</v>
+        <v>43489</v>
       </c>
       <c r="B32" t="s">
-        <v>232</v>
+        <v>230</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
       </c>
       <c r="D32">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F32">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
       <c r="H32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K32">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L32">
         <v>0</v>
       </c>
       <c r="M32">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N32">
         <v>4</v>
@@ -10976,13 +10961,13 @@
         <v>5</v>
       </c>
       <c r="P32">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q32">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="R32">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S32">
         <v>4</v>
@@ -10990,73 +10975,82 @@
       <c r="T32">
         <v>15</v>
       </c>
+      <c r="U32">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>43482</v>
+        <v>43487</v>
       </c>
       <c r="B33" t="s">
-        <v>233</v>
+        <v>231</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E33">
         <v>5</v>
       </c>
       <c r="F33">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G33">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
       <c r="H33">
         <v>5</v>
       </c>
       <c r="I33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K33">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
       <c r="M33">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N33">
         <v>4</v>
       </c>
       <c r="O33">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P33">
         <v>7</v>
       </c>
       <c r="Q33">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R33">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="S33">
         <v>4</v>
       </c>
       <c r="T33">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="U33">
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>43481</v>
+        <v>43482</v>
       </c>
       <c r="B34" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D34">
         <v>12</v>
@@ -11065,26 +11059,29 @@
         <v>5</v>
       </c>
       <c r="F34">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G34">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
       <c r="H34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J34">
         <v>4</v>
       </c>
       <c r="K34">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
       </c>
       <c r="M34">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N34">
         <v>4</v>
@@ -11093,84 +11090,201 @@
         <v>5</v>
       </c>
       <c r="P34">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q34">
         <v>12</v>
       </c>
       <c r="R34">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="S34">
         <v>4</v>
       </c>
       <c r="T34">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>43481</v>
+        <v>43482</v>
       </c>
       <c r="B35" t="s">
-        <v>235</v>
-      </c>
-      <c r="C35">
-        <v>6</v>
+        <v>233</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E35">
         <v>5</v>
       </c>
       <c r="F35">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="H35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I35">
         <v>4</v>
       </c>
       <c r="J35">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K35">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N35">
+        <v>4</v>
+      </c>
+      <c r="O35">
+        <v>4</v>
+      </c>
+      <c r="P35">
+        <v>7</v>
+      </c>
+      <c r="Q35">
+        <v>10</v>
+      </c>
+      <c r="R35">
+        <v>15</v>
+      </c>
+      <c r="S35">
+        <v>4</v>
+      </c>
+      <c r="T35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>43481</v>
+      </c>
+      <c r="B36" t="s">
+        <v>234</v>
+      </c>
+      <c r="D36">
+        <v>12</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H36">
+        <v>6</v>
+      </c>
+      <c r="I36">
+        <v>6</v>
+      </c>
+      <c r="J36">
+        <v>4</v>
+      </c>
+      <c r="K36">
+        <v>31</v>
+      </c>
+      <c r="M36">
+        <v>7</v>
+      </c>
+      <c r="N36">
+        <v>4</v>
+      </c>
+      <c r="O36">
+        <v>5</v>
+      </c>
+      <c r="P36">
+        <v>6</v>
+      </c>
+      <c r="Q36">
+        <v>12</v>
+      </c>
+      <c r="R36">
+        <v>10</v>
+      </c>
+      <c r="S36">
+        <v>4</v>
+      </c>
+      <c r="T36">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>43481</v>
+      </c>
+      <c r="B37" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>6</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>9</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <v>4</v>
+      </c>
+      <c r="J37">
+        <v>6</v>
+      </c>
+      <c r="K37">
+        <v>32</v>
+      </c>
+      <c r="L37">
         <v>0</v>
       </c>
-      <c r="O35">
-        <v>6</v>
-      </c>
-      <c r="P35">
-        <v>7</v>
-      </c>
-      <c r="Q35">
-        <v>6</v>
-      </c>
-      <c r="R35">
+      <c r="M37">
+        <v>8</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>6</v>
+      </c>
+      <c r="P37">
+        <v>7</v>
+      </c>
+      <c r="Q37">
+        <v>6</v>
+      </c>
+      <c r="R37">
         <v>14</v>
       </c>
-      <c r="S35">
+      <c r="S37">
         <v>0</v>
       </c>
-      <c r="T35">
+      <c r="T37">
         <v>13</v>
       </c>
-      <c r="U35">
+      <c r="U37">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small modifications to the polling graphs
</commit_message>
<xml_diff>
--- a/Data/polls.xlsx
+++ b/Data/polls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mac Tan\Desktop\Stuff\Elections\2019\Israel-2019\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E35A4A-1735-47BC-AE96-4A608338DBA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19785B47-1CB4-4F50-9B61-19DFED32B14A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-5733" windowWidth="26301" windowHeight="14305" activeTab="3" xr2:uid="{0DE1B94D-B05B-4FF7-9BF3-1803C0C1CFBD}"/>
+    <workbookView xWindow="25974" yWindow="-4904" windowWidth="26301" windowHeight="14305" activeTab="3" xr2:uid="{0DE1B94D-B05B-4FF7-9BF3-1803C0C1CFBD}"/>
   </bookViews>
   <sheets>
     <sheet name="2009" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="274">
   <si>
     <t>Channel 2[5]</t>
   </si>
@@ -851,6 +851,12 @@
   </si>
   <si>
     <t>Smith/Jerusalem Post[6]</t>
+  </si>
+  <si>
+    <t>Midgam/Channel 12[4]</t>
+  </si>
+  <si>
+    <t>Panel Project HaMidgam/Channel 13[5]</t>
   </si>
 </sst>
 </file>
@@ -9028,10 +9034,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CC49F9-512D-4648-8DF6-8D5ABA179EFE}">
-  <dimension ref="A1:V62"/>
+  <dimension ref="A1:V64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -9106,37 +9112,37 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>43546</v>
+        <v>43548</v>
       </c>
       <c r="B2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K2">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L2">
         <v>4</v>
@@ -9145,52 +9151,52 @@
         <v>5</v>
       </c>
       <c r="N2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P2">
         <v>7</v>
       </c>
       <c r="V2">
-        <f t="shared" ref="V2:V4" si="0">SUM(C2:P2)</f>
+        <f t="shared" ref="V2:V6" si="0">SUM(C2:P2)</f>
         <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>43546</v>
+        <v>43548</v>
       </c>
       <c r="B3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L3">
         <v>6</v>
@@ -9199,10 +9205,10 @@
         <v>5</v>
       </c>
       <c r="N3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P3">
         <v>6</v>
@@ -9217,46 +9223,46 @@
         <v>43546</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <v>30</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K4">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L4">
         <v>4</v>
       </c>
       <c r="M4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N4">
         <v>6</v>
       </c>
       <c r="O4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P4">
         <v>7</v>
@@ -9268,67 +9274,67 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>43544</v>
+        <v>43546</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J5">
         <v>4</v>
       </c>
       <c r="K5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V5">
-        <f>SUM(C5:P5)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>43544</v>
+        <v>43546</v>
       </c>
       <c r="B6" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -9337,10 +9343,10 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -9349,13 +9355,13 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K6">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M6">
         <v>6</v>
@@ -9364,37 +9370,37 @@
         <v>6</v>
       </c>
       <c r="O6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P6">
         <v>7</v>
       </c>
       <c r="V6">
-        <f t="shared" ref="V5:V35" si="1">SUM(C6:P6)</f>
-        <v>119</v>
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>43543</v>
+        <v>43544</v>
       </c>
       <c r="B7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H7">
         <v>4</v>
@@ -9403,10 +9409,10 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K7">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="L7">
         <v>4</v>
@@ -9415,55 +9421,55 @@
         <v>6</v>
       </c>
       <c r="N7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V7">
-        <f t="shared" si="1"/>
+        <f>SUM(C7:P7)</f>
         <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>43541</v>
+        <v>43544</v>
       </c>
       <c r="B8" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>4</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <v>9</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M8">
         <v>6</v>
@@ -9472,40 +9478,40 @@
         <v>6</v>
       </c>
       <c r="O8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V8">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <f t="shared" ref="V8:V37" si="1">SUM(C8:P8)</f>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>43538</v>
+        <v>43543</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G9">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -9514,10 +9520,10 @@
         <v>5</v>
       </c>
       <c r="K9">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M9">
         <v>6</v>
@@ -9526,10 +9532,10 @@
         <v>7</v>
       </c>
       <c r="O9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V9">
         <f t="shared" si="1"/>
@@ -9538,52 +9544,52 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>43538</v>
+        <v>43541</v>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10">
+        <v>30</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
         <v>31</v>
       </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>4</v>
-      </c>
-      <c r="K10">
-        <v>28</v>
-      </c>
       <c r="L10">
         <v>4</v>
       </c>
       <c r="M10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O10">
         <v>6</v>
       </c>
       <c r="P10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V10">
         <f t="shared" si="1"/>
@@ -9592,49 +9598,49 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>43537</v>
+        <v>43538</v>
       </c>
       <c r="B11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G11">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K11">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N11">
         <v>7</v>
       </c>
       <c r="O11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P11">
         <v>7</v>
@@ -9646,22 +9652,22 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>43535</v>
+        <v>43538</v>
       </c>
       <c r="B12" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C12">
         <v>7</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G12">
         <v>31</v>
@@ -9682,16 +9688,16 @@
         <v>4</v>
       </c>
       <c r="M12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N12">
         <v>7</v>
       </c>
       <c r="O12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V12">
         <f t="shared" si="1"/>
@@ -9700,46 +9706,46 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>43532</v>
+        <v>43537</v>
       </c>
       <c r="B13" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C13">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13">
         <v>10</v>
       </c>
       <c r="G13">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O13">
         <v>6</v>
@@ -9754,22 +9760,22 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>43531</v>
+        <v>43535</v>
       </c>
       <c r="B14" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G14">
         <v>31</v>
@@ -9781,7 +9787,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K14">
         <v>28</v>
@@ -9790,16 +9796,16 @@
         <v>4</v>
       </c>
       <c r="M14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O14">
         <v>5</v>
       </c>
       <c r="P14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V14">
         <f t="shared" si="1"/>
@@ -9808,22 +9814,22 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>43531</v>
+        <v>43532</v>
       </c>
       <c r="B15" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="C15">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G15">
         <v>33</v>
@@ -9835,25 +9841,25 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K15">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V15">
         <f t="shared" si="1"/>
@@ -9862,10 +9868,10 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>43529</v>
+        <v>43531</v>
       </c>
       <c r="B16" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C16">
         <v>8</v>
@@ -9874,16 +9880,16 @@
         <v>4</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -9892,16 +9898,16 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L16">
         <v>4</v>
       </c>
       <c r="M16">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O16">
         <v>5</v>
@@ -9916,52 +9922,52 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>43529</v>
+        <v>43531</v>
       </c>
       <c r="B17" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C17">
         <v>9</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G17">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H17">
         <v>4</v>
       </c>
       <c r="I17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="V17">
         <f t="shared" si="1"/>
@@ -9973,7 +9979,7 @@
         <v>43529</v>
       </c>
       <c r="B18" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C18">
         <v>8</v>
@@ -9982,13 +9988,13 @@
         <v>4</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G18">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -10003,23 +10009,23 @@
         <v>30</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M18">
         <v>5</v>
       </c>
       <c r="N18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P18">
         <v>7</v>
       </c>
       <c r="V18">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -10027,34 +10033,34 @@
         <v>43529</v>
       </c>
       <c r="B19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C19">
         <v>9</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K19">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -10063,13 +10069,13 @@
         <v>6</v>
       </c>
       <c r="N19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V19">
         <f t="shared" si="1"/>
@@ -10078,25 +10084,25 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>43527</v>
+        <v>43529</v>
       </c>
       <c r="B20" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G20">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H20">
         <v>5</v>
@@ -10114,10 +10120,10 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O20">
         <v>4</v>
@@ -10127,33 +10133,33 @@
       </c>
       <c r="V20">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>43525</v>
+        <v>43529</v>
       </c>
       <c r="B21" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C21">
         <v>9</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>6</v>
       </c>
       <c r="F21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G21">
         <v>36</v>
       </c>
       <c r="H21">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -10162,19 +10168,19 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N21">
         <v>7</v>
       </c>
       <c r="O21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P21">
         <v>7</v>
@@ -10186,25 +10192,25 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>43525</v>
+        <v>43527</v>
       </c>
       <c r="B22" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>6</v>
       </c>
       <c r="F22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H22">
         <v>5</v>
@@ -10216,19 +10222,19 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N22">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P22">
         <v>7</v>
@@ -10243,25 +10249,25 @@
         <v>43525</v>
       </c>
       <c r="B23" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E23">
         <v>6</v>
       </c>
       <c r="F23">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G23">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -10270,49 +10276,49 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N23">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O23">
         <v>6</v>
       </c>
       <c r="P23">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V23">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>43524</v>
+        <v>43525</v>
       </c>
       <c r="B24" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F24">
         <v>6</v>
       </c>
       <c r="G24">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H24">
         <v>5</v>
@@ -10321,7 +10327,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K24">
         <v>29</v>
@@ -10330,13 +10336,13 @@
         <v>0</v>
       </c>
       <c r="M24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N24">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P24">
         <v>7</v>
@@ -10348,28 +10354,28 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>43524</v>
+        <v>43525</v>
       </c>
       <c r="B25" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C25">
         <v>7</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E25">
         <v>6</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G25">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -10378,7 +10384,7 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -10387,7 +10393,7 @@
         <v>8</v>
       </c>
       <c r="N25">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O25">
         <v>6</v>
@@ -10397,33 +10403,33 @@
       </c>
       <c r="V25">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>43523</v>
+        <v>43524</v>
       </c>
       <c r="B26" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C26">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F26">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G26">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -10438,13 +10444,13 @@
         <v>0</v>
       </c>
       <c r="M26">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N26">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P26">
         <v>7</v>
@@ -10456,10 +10462,10 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>43520</v>
+        <v>43524</v>
       </c>
       <c r="B27" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C27">
         <v>7</v>
@@ -10468,16 +10474,16 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G27">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -10486,22 +10492,22 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N27">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V27">
         <f t="shared" si="1"/>
@@ -10510,25 +10516,25 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>43520</v>
+        <v>43523</v>
       </c>
       <c r="B28" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C28">
         <v>7</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28">
         <v>4</v>
       </c>
       <c r="F28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G28">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H28">
         <v>4</v>
@@ -10546,13 +10552,13 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N28">
         <v>5</v>
       </c>
       <c r="O28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P28">
         <v>7</v>
@@ -10564,67 +10570,67 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>43518</v>
+        <v>43520</v>
       </c>
       <c r="B29" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D29">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F29">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G29">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H29">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
       <c r="J29">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K29">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N29">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O29">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V29">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>43517</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>242</v>
+        <v>43520</v>
+      </c>
+      <c r="B30" t="s">
+        <v>250</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -10633,7 +10639,7 @@
         <v>4</v>
       </c>
       <c r="F30">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G30">
         <v>35</v>
@@ -10654,10 +10660,10 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O30">
         <v>5</v>
@@ -10672,25 +10678,25 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>43517</v>
+        <v>43518</v>
       </c>
       <c r="B31" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C31">
         <v>6</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E31">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F31">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G31">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H31">
         <v>4</v>
@@ -10702,7 +10708,7 @@
         <v>4</v>
       </c>
       <c r="K31">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -10711,31 +10717,31 @@
         <v>6</v>
       </c>
       <c r="N31">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P31">
         <v>6</v>
       </c>
       <c r="V31">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43517</v>
       </c>
-      <c r="B32" t="s">
-        <v>244</v>
+      <c r="B32" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="C32">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -10747,16 +10753,16 @@
         <v>35</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I32">
         <v>0</v>
       </c>
       <c r="J32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K32">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -10783,13 +10789,13 @@
         <v>43517</v>
       </c>
       <c r="B33" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C33">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -10798,31 +10804,31 @@
         <v>8</v>
       </c>
       <c r="G33">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K33">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
       <c r="M33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P33">
         <v>6</v>
@@ -10837,43 +10843,43 @@
         <v>43517</v>
       </c>
       <c r="B34" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D34">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <v>4</v>
       </c>
       <c r="F34">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G34">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H34">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K34">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L34">
         <v>0</v>
       </c>
       <c r="M34">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N34">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O34">
         <v>5</v>
@@ -10891,25 +10897,25 @@
         <v>43517</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C35">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E35">
         <v>4</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G35">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -10918,22 +10924,22 @@
         <v>5</v>
       </c>
       <c r="K35">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N35">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O35">
         <v>6</v>
       </c>
       <c r="P35">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V35">
         <f t="shared" si="1"/>
@@ -10942,82 +10948,70 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="B36" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="C36">
         <v>6</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F36">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G36">
-        <f>R36+T36</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H36">
         <v>4</v>
       </c>
       <c r="I36">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K36">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P36">
         <v>7</v>
       </c>
-      <c r="Q36">
-        <v>5</v>
-      </c>
-      <c r="R36">
-        <v>13</v>
-      </c>
-      <c r="S36">
-        <v>5</v>
-      </c>
-      <c r="T36">
-        <v>19</v>
-      </c>
-      <c r="U36">
-        <v>6</v>
+      <c r="V36">
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>43513</v>
+        <v>43517</v>
       </c>
       <c r="B37" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -11026,8 +11020,7 @@
         <v>5</v>
       </c>
       <c r="G37">
-        <f t="shared" ref="G37:G62" si="2">R37+T37</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H37">
         <v>4</v>
@@ -11036,205 +11029,194 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K37">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L37">
         <v>0</v>
       </c>
       <c r="M37">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N37">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O37">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P37">
-        <v>6</v>
-      </c>
-      <c r="Q37">
-        <v>7</v>
-      </c>
-      <c r="R37">
-        <v>10</v>
-      </c>
-      <c r="S37">
-        <v>5</v>
-      </c>
-      <c r="T37">
-        <v>24</v>
-      </c>
-      <c r="U37">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
+        <v>43516</v>
+      </c>
+      <c r="B38" t="s">
+        <v>237</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>9</v>
+      </c>
+      <c r="G38">
+        <f>R38+T38</f>
+        <v>32</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>4</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>31</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>8</v>
+      </c>
+      <c r="N38">
+        <v>5</v>
+      </c>
+      <c r="O38">
+        <v>4</v>
+      </c>
+      <c r="P38">
+        <v>7</v>
+      </c>
+      <c r="Q38">
+        <v>5</v>
+      </c>
+      <c r="R38">
+        <v>13</v>
+      </c>
+      <c r="S38">
+        <v>5</v>
+      </c>
+      <c r="T38">
+        <v>19</v>
+      </c>
+      <c r="U38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
         <v>43513</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39">
+        <f t="shared" ref="G39:G64" si="2">R39+T39</f>
+        <v>34</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>4</v>
+      </c>
+      <c r="K39">
+        <v>32</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>9</v>
+      </c>
+      <c r="N39">
+        <v>5</v>
+      </c>
+      <c r="O39">
+        <v>4</v>
+      </c>
+      <c r="P39">
+        <v>6</v>
+      </c>
+      <c r="Q39">
+        <v>7</v>
+      </c>
+      <c r="R39">
+        <v>10</v>
+      </c>
+      <c r="S39">
+        <v>5</v>
+      </c>
+      <c r="T39">
+        <v>24</v>
+      </c>
+      <c r="U39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>43513</v>
+      </c>
+      <c r="B40" t="s">
         <v>213</v>
       </c>
-      <c r="C38">
-        <v>7</v>
-      </c>
-      <c r="D38">
-        <v>5</v>
-      </c>
-      <c r="E38">
-        <v>5</v>
-      </c>
-      <c r="F38">
-        <v>10</v>
-      </c>
-      <c r="G38">
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+      <c r="G40">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H38">
-        <v>5</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>4</v>
-      </c>
-      <c r="K38">
-        <v>30</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>7</v>
-      </c>
-      <c r="N38">
-        <v>4</v>
-      </c>
-      <c r="O38">
-        <v>6</v>
-      </c>
-      <c r="P38">
-        <v>7</v>
-      </c>
-      <c r="Q38">
-        <v>5</v>
-      </c>
-      <c r="R38">
-        <v>12</v>
-      </c>
-      <c r="S38">
-        <v>4</v>
-      </c>
-      <c r="T38">
-        <v>18</v>
-      </c>
-      <c r="U38">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>43512</v>
-      </c>
-      <c r="B39" t="s">
-        <v>214</v>
-      </c>
-      <c r="C39">
-        <v>6</v>
-      </c>
-      <c r="D39">
-        <v>6</v>
-      </c>
-      <c r="E39">
-        <v>5</v>
-      </c>
-      <c r="F39">
-        <v>10</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="H39">
-        <v>4</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>5</v>
-      </c>
-      <c r="K39">
-        <v>30</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39">
-        <v>8</v>
-      </c>
-      <c r="N39">
-        <v>5</v>
-      </c>
-      <c r="O39">
-        <v>5</v>
-      </c>
-      <c r="P39">
-        <v>6</v>
-      </c>
-      <c r="Q39">
-        <v>6</v>
-      </c>
-      <c r="R39">
-        <v>10</v>
-      </c>
-      <c r="S39">
-        <v>5</v>
-      </c>
-      <c r="T39">
-        <v>20</v>
-      </c>
-      <c r="U39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>43509</v>
-      </c>
-      <c r="B40" t="s">
-        <v>215</v>
-      </c>
-      <c r="C40">
-        <v>6</v>
-      </c>
-      <c r="D40">
-        <v>6</v>
-      </c>
-      <c r="E40">
-        <v>4</v>
-      </c>
-      <c r="F40">
-        <v>11</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
       <c r="H40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I40">
         <v>0</v>
       </c>
       <c r="J40">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K40">
         <v>30</v>
@@ -11243,64 +11225,64 @@
         <v>0</v>
       </c>
       <c r="M40">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N40">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O40">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P40">
         <v>7</v>
       </c>
       <c r="Q40">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R40">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S40">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T40">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="U40">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>43508</v>
+        <v>43512</v>
       </c>
       <c r="B41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C41">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E41">
         <v>5</v>
       </c>
       <c r="F41">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G41">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="H41">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I41">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K41">
         <v>30</v>
@@ -11309,79 +11291,79 @@
         <v>0</v>
       </c>
       <c r="M41">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N41">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P41">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R41">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S41">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T41">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U41">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>43508</v>
+        <v>43509</v>
       </c>
       <c r="B42" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D42">
         <v>6</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G42">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I42">
         <v>0</v>
       </c>
       <c r="J42">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K42">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L42">
         <v>0</v>
       </c>
       <c r="M42">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N42">
         <v>0</v>
       </c>
       <c r="O42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P42">
         <v>7</v>
@@ -11396,18 +11378,18 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U42">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>43504</v>
+        <v>43508</v>
       </c>
       <c r="B43" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C43">
         <v>7</v>
@@ -11419,32 +11401,32 @@
         <v>5</v>
       </c>
       <c r="F43">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G43">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K43">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L43">
         <v>0</v>
       </c>
       <c r="M43">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O43">
         <v>6</v>
@@ -11459,10 +11441,10 @@
         <v>11</v>
       </c>
       <c r="S43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T43">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="U43">
         <v>7</v>
@@ -11470,26 +11452,26 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>43503</v>
+        <v>43508</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="C44">
         <v>7</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E44">
         <v>5</v>
       </c>
       <c r="F44">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G44">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H44">
         <v>5</v>
@@ -11498,7 +11480,7 @@
         <v>0</v>
       </c>
       <c r="J44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K44">
         <v>32</v>
@@ -11519,7 +11501,7 @@
         <v>7</v>
       </c>
       <c r="Q44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R44">
         <v>11</v>
@@ -11528,7 +11510,7 @@
         <v>0</v>
       </c>
       <c r="T44">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U44">
         <v>7</v>
@@ -11536,35 +11518,35 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>43503</v>
+        <v>43504</v>
       </c>
       <c r="B45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D45">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F45">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G45">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="H45">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I45">
         <v>0</v>
       </c>
       <c r="J45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K45">
         <v>32</v>
@@ -11573,31 +11555,31 @@
         <v>0</v>
       </c>
       <c r="M45">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P45">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q45">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R45">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T45">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U45">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
@@ -11605,23 +11587,23 @@
         <v>43503</v>
       </c>
       <c r="B46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C46">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D46">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E46">
         <v>5</v>
       </c>
       <c r="F46">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G46">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H46">
         <v>5</v>
@@ -11630,40 +11612,40 @@
         <v>0</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K46">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L46">
         <v>0</v>
       </c>
       <c r="M46">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N46">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P46">
         <v>7</v>
       </c>
       <c r="Q46">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R46">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S46">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T46">
         <v>22</v>
       </c>
       <c r="U46">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
@@ -11671,125 +11653,125 @@
         <v>43503</v>
       </c>
       <c r="B47" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D47">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E47">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F47">
         <v>5</v>
       </c>
       <c r="G47">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I47">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K47">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L47">
         <v>0</v>
       </c>
       <c r="M47">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N47">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O47">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P47">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q47">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="R47">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="S47">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T47">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="U47">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>43502</v>
+        <v>43503</v>
       </c>
       <c r="B48" t="s">
-        <v>221</v>
+        <v>154</v>
       </c>
       <c r="C48">
         <v>6</v>
       </c>
       <c r="D48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48">
         <v>5</v>
       </c>
       <c r="G48">
         <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
         <v>34</v>
       </c>
-      <c r="H48">
-        <v>5</v>
-      </c>
-      <c r="I48">
-        <v>4</v>
-      </c>
-      <c r="J48">
-        <v>5</v>
-      </c>
-      <c r="K48">
-        <v>30</v>
-      </c>
       <c r="L48">
         <v>0</v>
       </c>
       <c r="M48">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N48">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R48">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S48">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T48">
         <v>22</v>
@@ -11800,38 +11782,38 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>43502</v>
+        <v>43503</v>
       </c>
       <c r="B49" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C49">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G49">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H49">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J49">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K49">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -11840,52 +11822,52 @@
         <v>7</v>
       </c>
       <c r="N49">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P49">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q49">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="R49">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="S49">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T49">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U49">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>43500</v>
+        <v>43502</v>
       </c>
       <c r="B50" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F50">
         <v>5</v>
       </c>
       <c r="G50">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H50">
         <v>5</v>
@@ -11903,10 +11885,10 @@
         <v>0</v>
       </c>
       <c r="M50">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N50">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O50">
         <v>5</v>
@@ -11915,99 +11897,99 @@
         <v>6</v>
       </c>
       <c r="Q50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R50">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S50">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T50">
         <v>22</v>
       </c>
       <c r="U50">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>43497</v>
+        <v>43502</v>
       </c>
       <c r="B51" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C51">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E51">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51">
         <v>6</v>
       </c>
       <c r="G51">
         <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H51">
+        <v>4</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>5</v>
+      </c>
+      <c r="K51">
         <v>32</v>
       </c>
-      <c r="H51">
-        <v>5</v>
-      </c>
-      <c r="I51">
-        <v>4</v>
-      </c>
-      <c r="J51">
-        <v>5</v>
-      </c>
-      <c r="K51">
-        <v>31</v>
-      </c>
       <c r="L51">
         <v>0</v>
       </c>
       <c r="M51">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P51">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q51">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R51">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T51">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="U51">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>43496</v>
+        <v>43500</v>
       </c>
       <c r="B52" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D52">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -12017,7 +11999,7 @@
       </c>
       <c r="G52">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H52">
         <v>5</v>
@@ -12026,76 +12008,76 @@
         <v>4</v>
       </c>
       <c r="J52">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K52">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L52">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M52">
         <v>7</v>
       </c>
       <c r="N52">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P52">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q52">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R52">
         <v>9</v>
       </c>
       <c r="S52">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T52">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="U52">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>43495</v>
+        <v>43497</v>
       </c>
       <c r="B53" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C53">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D53">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E53">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F53">
         <v>6</v>
       </c>
       <c r="G53">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H53">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I53">
         <v>4</v>
       </c>
       <c r="J53">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K53">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L53">
         <v>0</v>
@@ -12107,49 +12089,49 @@
         <v>4</v>
       </c>
       <c r="O53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P53">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q53">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R53">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S53">
         <v>4</v>
       </c>
       <c r="T53">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="U53">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>43495</v>
+        <v>43496</v>
       </c>
       <c r="B54" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C54">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E54">
         <v>4</v>
       </c>
       <c r="F54">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G54">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H54">
         <v>5</v>
@@ -12158,40 +12140,40 @@
         <v>4</v>
       </c>
       <c r="J54">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K54">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L54">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M54">
         <v>7</v>
       </c>
       <c r="N54">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O54">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P54">
         <v>7</v>
       </c>
       <c r="Q54">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R54">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S54">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T54">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U54">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -12199,47 +12181,47 @@
         <v>43495</v>
       </c>
       <c r="B55" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C55">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D55">
         <v>6</v>
       </c>
       <c r="E55">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F55">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G55">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H55">
         <v>4</v>
       </c>
       <c r="I55">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J55">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K55">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L55">
         <v>0</v>
       </c>
       <c r="M55">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N55">
         <v>4</v>
       </c>
       <c r="O55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P55">
         <v>6</v>
@@ -12254,10 +12236,10 @@
         <v>4</v>
       </c>
       <c r="T55">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U55">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
@@ -12265,23 +12247,23 @@
         <v>43495</v>
       </c>
       <c r="B56" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C56">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E56">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G56">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H56">
         <v>5</v>
@@ -12290,10 +12272,10 @@
         <v>4</v>
       </c>
       <c r="J56">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K56">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L56">
         <v>0</v>
@@ -12305,33 +12287,33 @@
         <v>4</v>
       </c>
       <c r="O56">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P56">
         <v>7</v>
       </c>
       <c r="Q56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R56">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S56">
         <v>4</v>
       </c>
       <c r="T56">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="U56">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>43489</v>
+        <v>43495</v>
       </c>
       <c r="B57" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C57">
         <v>6</v>
@@ -12343,17 +12325,17 @@
         <v>6</v>
       </c>
       <c r="F57">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G57">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H57">
         <v>4</v>
       </c>
       <c r="I57">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J57">
         <v>5</v>
@@ -12371,7 +12353,7 @@
         <v>4</v>
       </c>
       <c r="O57">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P57">
         <v>6</v>
@@ -12380,13 +12362,13 @@
         <v>6</v>
       </c>
       <c r="R57">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S57">
         <v>4</v>
       </c>
       <c r="T57">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="U57">
         <v>6</v>
@@ -12394,32 +12376,32 @@
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>43487</v>
+        <v>43495</v>
       </c>
       <c r="B58" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C58">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D58">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E58">
         <v>5</v>
       </c>
       <c r="F58">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G58">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H58">
         <v>5</v>
       </c>
       <c r="I58">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J58">
         <v>5</v>
@@ -12437,64 +12419,67 @@
         <v>4</v>
       </c>
       <c r="O58">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P58">
         <v>7</v>
       </c>
       <c r="Q58">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R58">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S58">
         <v>4</v>
       </c>
       <c r="T58">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="U58">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>43482</v>
+        <v>43489</v>
       </c>
       <c r="B59" t="s">
-        <v>232</v>
+        <v>230</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
       </c>
       <c r="D59">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E59">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F59">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G59">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J59">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K59">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L59">
         <v>0</v>
       </c>
       <c r="M59">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N59">
         <v>4</v>
@@ -12503,13 +12488,13 @@
         <v>5</v>
       </c>
       <c r="P59">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q59">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="R59">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S59">
         <v>4</v>
@@ -12517,73 +12502,82 @@
       <c r="T59">
         <v>15</v>
       </c>
+      <c r="U59">
+        <v>6</v>
+      </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>43482</v>
+        <v>43487</v>
       </c>
       <c r="B60" t="s">
-        <v>233</v>
+        <v>231</v>
+      </c>
+      <c r="C60">
+        <v>6</v>
       </c>
       <c r="D60">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E60">
         <v>5</v>
       </c>
       <c r="F60">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G60">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H60">
         <v>5</v>
       </c>
       <c r="I60">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J60">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K60">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L60">
         <v>0</v>
       </c>
       <c r="M60">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N60">
         <v>4</v>
       </c>
       <c r="O60">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P60">
         <v>7</v>
       </c>
       <c r="Q60">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R60">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="S60">
         <v>4</v>
       </c>
       <c r="T60">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="U60">
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>43481</v>
+        <v>43482</v>
       </c>
       <c r="B61" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D61">
         <v>12</v>
@@ -12592,26 +12586,29 @@
         <v>5</v>
       </c>
       <c r="F61">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G61">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H61">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I61">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J61">
         <v>4</v>
       </c>
       <c r="K61">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
       </c>
       <c r="M61">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N61">
         <v>4</v>
@@ -12620,84 +12617,201 @@
         <v>5</v>
       </c>
       <c r="P61">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q61">
         <v>12</v>
       </c>
       <c r="R61">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="S61">
         <v>4</v>
       </c>
       <c r="T61">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>43481</v>
+        <v>43482</v>
       </c>
       <c r="B62" t="s">
-        <v>235</v>
-      </c>
-      <c r="C62">
-        <v>6</v>
+        <v>233</v>
       </c>
       <c r="D62">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E62">
         <v>5</v>
       </c>
       <c r="F62">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G62">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="H62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I62">
         <v>4</v>
       </c>
       <c r="J62">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K62">
+        <v>33</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>9</v>
+      </c>
+      <c r="N62">
+        <v>4</v>
+      </c>
+      <c r="O62">
+        <v>4</v>
+      </c>
+      <c r="P62">
+        <v>7</v>
+      </c>
+      <c r="Q62">
+        <v>10</v>
+      </c>
+      <c r="R62">
+        <v>15</v>
+      </c>
+      <c r="S62">
+        <v>4</v>
+      </c>
+      <c r="T62">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>43481</v>
+      </c>
+      <c r="B63" t="s">
+        <v>234</v>
+      </c>
+      <c r="D63">
+        <v>12</v>
+      </c>
+      <c r="E63">
+        <v>5</v>
+      </c>
+      <c r="F63">
+        <v>7</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="H63">
+        <v>6</v>
+      </c>
+      <c r="I63">
+        <v>6</v>
+      </c>
+      <c r="J63">
+        <v>4</v>
+      </c>
+      <c r="K63">
+        <v>31</v>
+      </c>
+      <c r="M63">
+        <v>7</v>
+      </c>
+      <c r="N63">
+        <v>4</v>
+      </c>
+      <c r="O63">
+        <v>5</v>
+      </c>
+      <c r="P63">
+        <v>6</v>
+      </c>
+      <c r="Q63">
+        <v>12</v>
+      </c>
+      <c r="R63">
+        <v>10</v>
+      </c>
+      <c r="S63">
+        <v>4</v>
+      </c>
+      <c r="T63">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>43481</v>
+      </c>
+      <c r="B64" t="s">
+        <v>235</v>
+      </c>
+      <c r="C64">
+        <v>6</v>
+      </c>
+      <c r="D64">
+        <v>6</v>
+      </c>
+      <c r="E64">
+        <v>5</v>
+      </c>
+      <c r="F64">
+        <v>9</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="H64">
+        <v>4</v>
+      </c>
+      <c r="I64">
+        <v>4</v>
+      </c>
+      <c r="J64">
+        <v>6</v>
+      </c>
+      <c r="K64">
         <v>32</v>
       </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-      <c r="M62">
-        <v>8</v>
-      </c>
-      <c r="N62">
-        <v>0</v>
-      </c>
-      <c r="O62">
-        <v>6</v>
-      </c>
-      <c r="P62">
-        <v>7</v>
-      </c>
-      <c r="Q62">
-        <v>6</v>
-      </c>
-      <c r="R62">
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>8</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>6</v>
+      </c>
+      <c r="P64">
+        <v>7</v>
+      </c>
+      <c r="Q64">
+        <v>6</v>
+      </c>
+      <c r="R64">
         <v>14</v>
       </c>
-      <c r="S62">
-        <v>0</v>
-      </c>
-      <c r="T62">
+      <c r="S64">
+        <v>0</v>
+      </c>
+      <c r="T64">
         <v>13</v>
       </c>
-      <c r="U62">
+      <c r="U64">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated for 26 Mar 2019 polls
</commit_message>
<xml_diff>
--- a/Data/polls.xlsx
+++ b/Data/polls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mac Tan\Desktop\Stuff\Elections\2019\Israel-2019\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19785B47-1CB4-4F50-9B61-19DFED32B14A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E274BEFC-0C73-4EC9-80A2-33B74B7573C3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-4904" windowWidth="26301" windowHeight="14305" activeTab="3" xr2:uid="{0DE1B94D-B05B-4FF7-9BF3-1803C0C1CFBD}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="3" xr2:uid="{0DE1B94D-B05B-4FF7-9BF3-1803C0C1CFBD}"/>
   </bookViews>
   <sheets>
     <sheet name="2009" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="275">
   <si>
     <t>Channel 2[5]</t>
   </si>
@@ -857,6 +857,9 @@
   </si>
   <si>
     <t>Panel Project HaMidgam/Channel 13[5]</t>
+  </si>
+  <si>
+    <t>Midgam/Army Radio[4]</t>
   </si>
 </sst>
 </file>
@@ -9034,10 +9037,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CC49F9-512D-4648-8DF6-8D5ABA179EFE}">
-  <dimension ref="A1:V64"/>
+  <dimension ref="A1:V66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -9112,28 +9115,28 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>43548</v>
+        <v>43550</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -9160,34 +9163,34 @@
         <v>7</v>
       </c>
       <c r="V2">
-        <f t="shared" ref="V2:V6" si="0">SUM(C2:P2)</f>
+        <f t="shared" ref="V2:V8" si="0">SUM(C2:P2)</f>
         <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>43548</v>
+        <v>43550</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="C3">
         <v>7</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -9202,16 +9205,16 @@
         <v>6</v>
       </c>
       <c r="M3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V3">
         <f t="shared" si="0"/>
@@ -9220,37 +9223,37 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>43546</v>
+        <v>43548</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K4">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L4">
         <v>4</v>
@@ -9259,10 +9262,10 @@
         <v>5</v>
       </c>
       <c r="N4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P4">
         <v>7</v>
@@ -9274,37 +9277,37 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>43546</v>
+        <v>43548</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L5">
         <v>6</v>
@@ -9313,10 +9316,10 @@
         <v>5</v>
       </c>
       <c r="N5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P5">
         <v>6</v>
@@ -9331,46 +9334,46 @@
         <v>43546</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6">
         <v>30</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K6">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L6">
         <v>4</v>
       </c>
       <c r="M6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N6">
         <v>6</v>
       </c>
       <c r="O6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P6">
         <v>7</v>
@@ -9382,67 +9385,67 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>43544</v>
+        <v>43546</v>
       </c>
       <c r="B7" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H7">
         <v>4</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J7">
         <v>4</v>
       </c>
       <c r="K7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V7">
-        <f>SUM(C7:P7)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>43544</v>
+        <v>43546</v>
       </c>
       <c r="B8" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -9451,10 +9454,10 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8">
         <v>5</v>
@@ -9463,13 +9466,13 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K8">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M8">
         <v>6</v>
@@ -9478,37 +9481,37 @@
         <v>6</v>
       </c>
       <c r="O8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P8">
         <v>7</v>
       </c>
       <c r="V8">
-        <f t="shared" ref="V8:V37" si="1">SUM(C8:P8)</f>
-        <v>119</v>
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>43543</v>
+        <v>43544</v>
       </c>
       <c r="B9" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G9">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H9">
         <v>4</v>
@@ -9517,10 +9520,10 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K9">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="L9">
         <v>4</v>
@@ -9529,55 +9532,55 @@
         <v>6</v>
       </c>
       <c r="N9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V9">
-        <f t="shared" si="1"/>
+        <f>SUM(C9:P9)</f>
         <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>43541</v>
+        <v>43544</v>
       </c>
       <c r="B10" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M10">
         <v>6</v>
@@ -9586,40 +9589,40 @@
         <v>6</v>
       </c>
       <c r="O10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V10">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <f t="shared" ref="V10:V39" si="1">SUM(C10:P10)</f>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>43538</v>
+        <v>43543</v>
       </c>
       <c r="B11" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G11">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -9628,10 +9631,10 @@
         <v>5</v>
       </c>
       <c r="K11">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M11">
         <v>6</v>
@@ -9640,10 +9643,10 @@
         <v>7</v>
       </c>
       <c r="O11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V11">
         <f t="shared" si="1"/>
@@ -9652,52 +9655,52 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>43538</v>
+        <v>43541</v>
       </c>
       <c r="B12" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12">
+        <v>30</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
         <v>31</v>
       </c>
-      <c r="H12">
-        <v>4</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
-      <c r="K12">
-        <v>28</v>
-      </c>
       <c r="L12">
         <v>4</v>
       </c>
       <c r="M12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O12">
         <v>6</v>
       </c>
       <c r="P12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V12">
         <f t="shared" si="1"/>
@@ -9706,49 +9709,49 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>43537</v>
+        <v>43538</v>
       </c>
       <c r="B13" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="C13">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G13">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K13">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N13">
         <v>7</v>
       </c>
       <c r="O13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P13">
         <v>7</v>
@@ -9760,22 +9763,22 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>43535</v>
+        <v>43538</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C14">
         <v>7</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F14">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G14">
         <v>31</v>
@@ -9796,16 +9799,16 @@
         <v>4</v>
       </c>
       <c r="M14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N14">
         <v>7</v>
       </c>
       <c r="O14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V14">
         <f t="shared" si="1"/>
@@ -9814,46 +9817,46 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>43532</v>
+        <v>43537</v>
       </c>
       <c r="B15" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F15">
         <v>10</v>
       </c>
       <c r="G15">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O15">
         <v>6</v>
@@ -9868,22 +9871,22 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>43531</v>
+        <v>43535</v>
       </c>
       <c r="B16" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G16">
         <v>31</v>
@@ -9895,7 +9898,7 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K16">
         <v>28</v>
@@ -9904,16 +9907,16 @@
         <v>4</v>
       </c>
       <c r="M16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O16">
         <v>5</v>
       </c>
       <c r="P16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V16">
         <f t="shared" si="1"/>
@@ -9922,22 +9925,22 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>43531</v>
+        <v>43532</v>
       </c>
       <c r="B17" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="C17">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F17">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G17">
         <v>33</v>
@@ -9949,25 +9952,25 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K17">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N17">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V17">
         <f t="shared" si="1"/>
@@ -9976,10 +9979,10 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>43529</v>
+        <v>43531</v>
       </c>
       <c r="B18" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C18">
         <v>8</v>
@@ -9988,16 +9991,16 @@
         <v>4</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -10006,16 +10009,16 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L18">
         <v>4</v>
       </c>
       <c r="M18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N18">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O18">
         <v>5</v>
@@ -10030,52 +10033,52 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>43529</v>
+        <v>43531</v>
       </c>
       <c r="B19" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C19">
         <v>9</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G19">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H19">
         <v>4</v>
       </c>
       <c r="I19">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="V19">
         <f t="shared" si="1"/>
@@ -10087,7 +10090,7 @@
         <v>43529</v>
       </c>
       <c r="B20" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -10096,13 +10099,13 @@
         <v>4</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G20">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20">
         <v>5</v>
@@ -10117,23 +10120,23 @@
         <v>30</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M20">
         <v>5</v>
       </c>
       <c r="N20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P20">
         <v>7</v>
       </c>
       <c r="V20">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -10141,34 +10144,34 @@
         <v>43529</v>
       </c>
       <c r="B21" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C21">
         <v>9</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G21">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K21">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -10177,13 +10180,13 @@
         <v>6</v>
       </c>
       <c r="N21">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P21">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V21">
         <f t="shared" si="1"/>
@@ -10192,25 +10195,25 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>43527</v>
+        <v>43529</v>
       </c>
       <c r="B22" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G22">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H22">
         <v>5</v>
@@ -10228,10 +10231,10 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O22">
         <v>4</v>
@@ -10241,33 +10244,33 @@
       </c>
       <c r="V22">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>43525</v>
+        <v>43529</v>
       </c>
       <c r="B23" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C23">
         <v>9</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>6</v>
       </c>
       <c r="F23">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G23">
         <v>36</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -10276,19 +10279,19 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N23">
         <v>7</v>
       </c>
       <c r="O23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P23">
         <v>7</v>
@@ -10300,25 +10303,25 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>43525</v>
+        <v>43527</v>
       </c>
       <c r="B24" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C24">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>6</v>
       </c>
       <c r="F24">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G24">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H24">
         <v>5</v>
@@ -10330,19 +10333,19 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N24">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O24">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P24">
         <v>7</v>
@@ -10357,25 +10360,25 @@
         <v>43525</v>
       </c>
       <c r="B25" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>6</v>
       </c>
       <c r="F25">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -10384,49 +10387,49 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N25">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O25">
         <v>6</v>
       </c>
       <c r="P25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V25">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>43524</v>
+        <v>43525</v>
       </c>
       <c r="B26" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C26">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F26">
         <v>6</v>
       </c>
       <c r="G26">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H26">
         <v>5</v>
@@ -10435,7 +10438,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K26">
         <v>29</v>
@@ -10444,13 +10447,13 @@
         <v>0</v>
       </c>
       <c r="M26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N26">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P26">
         <v>7</v>
@@ -10462,28 +10465,28 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>43524</v>
+        <v>43525</v>
       </c>
       <c r="B27" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C27">
         <v>7</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E27">
         <v>6</v>
       </c>
       <c r="F27">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G27">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -10492,7 +10495,7 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -10501,7 +10504,7 @@
         <v>8</v>
       </c>
       <c r="N27">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O27">
         <v>6</v>
@@ -10511,33 +10514,33 @@
       </c>
       <c r="V27">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>43523</v>
+        <v>43524</v>
       </c>
       <c r="B28" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C28">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F28">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G28">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -10552,13 +10555,13 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N28">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P28">
         <v>7</v>
@@ -10570,10 +10573,10 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>43520</v>
+        <v>43524</v>
       </c>
       <c r="B29" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C29">
         <v>7</v>
@@ -10582,16 +10585,16 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G29">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -10600,22 +10603,22 @@
         <v>0</v>
       </c>
       <c r="K29">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N29">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V29">
         <f t="shared" si="1"/>
@@ -10624,25 +10627,25 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>43520</v>
+        <v>43523</v>
       </c>
       <c r="B30" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C30">
         <v>7</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E30">
         <v>4</v>
       </c>
       <c r="F30">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G30">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H30">
         <v>4</v>
@@ -10660,13 +10663,13 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N30">
         <v>5</v>
       </c>
       <c r="O30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P30">
         <v>7</v>
@@ -10678,67 +10681,67 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>43518</v>
+        <v>43520</v>
       </c>
       <c r="B31" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D31">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G31">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H31">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K31">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L31">
         <v>0</v>
       </c>
       <c r="M31">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N31">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O31">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V31">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>43517</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>242</v>
+        <v>43520</v>
+      </c>
+      <c r="B32" t="s">
+        <v>250</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D32">
         <v>5</v>
@@ -10747,7 +10750,7 @@
         <v>4</v>
       </c>
       <c r="F32">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G32">
         <v>35</v>
@@ -10768,10 +10771,10 @@
         <v>0</v>
       </c>
       <c r="M32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O32">
         <v>5</v>
@@ -10786,25 +10789,25 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>43517</v>
+        <v>43518</v>
       </c>
       <c r="B33" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C33">
         <v>6</v>
       </c>
       <c r="D33">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G33">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H33">
         <v>4</v>
@@ -10816,7 +10819,7 @@
         <v>4</v>
       </c>
       <c r="K33">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -10825,31 +10828,31 @@
         <v>6</v>
       </c>
       <c r="N33">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P33">
         <v>6</v>
       </c>
       <c r="V33">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43517</v>
       </c>
-      <c r="B34" t="s">
-        <v>244</v>
+      <c r="B34" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="C34">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -10861,16 +10864,16 @@
         <v>35</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K34">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -10897,13 +10900,13 @@
         <v>43517</v>
       </c>
       <c r="B35" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C35">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E35">
         <v>4</v>
@@ -10912,31 +10915,31 @@
         <v>8</v>
       </c>
       <c r="G35">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I35">
         <v>0</v>
       </c>
       <c r="J35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K35">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P35">
         <v>6</v>
@@ -10951,43 +10954,43 @@
         <v>43517</v>
       </c>
       <c r="B36" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C36">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D36">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>4</v>
       </c>
       <c r="F36">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G36">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H36">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
       <c r="J36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K36">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O36">
         <v>5</v>
@@ -11005,25 +11008,25 @@
         <v>43517</v>
       </c>
       <c r="B37" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C37">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E37">
         <v>4</v>
       </c>
       <c r="F37">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H37">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -11032,22 +11035,22 @@
         <v>5</v>
       </c>
       <c r="K37">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L37">
         <v>0</v>
       </c>
       <c r="M37">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O37">
         <v>6</v>
       </c>
       <c r="P37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V37">
         <f t="shared" si="1"/>
@@ -11056,82 +11059,70 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="B38" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="C38">
         <v>6</v>
       </c>
       <c r="D38">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G38">
-        <f>R38+T38</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H38">
         <v>4</v>
       </c>
       <c r="I38">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K38">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P38">
         <v>7</v>
       </c>
-      <c r="Q38">
-        <v>5</v>
-      </c>
-      <c r="R38">
-        <v>13</v>
-      </c>
-      <c r="S38">
-        <v>5</v>
-      </c>
-      <c r="T38">
-        <v>19</v>
-      </c>
-      <c r="U38">
-        <v>6</v>
+      <c r="V38">
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>43513</v>
+        <v>43517</v>
       </c>
       <c r="B39" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="C39">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -11140,8 +11131,7 @@
         <v>5</v>
       </c>
       <c r="G39">
-        <f t="shared" ref="G39:G64" si="2">R39+T39</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H39">
         <v>4</v>
@@ -11150,205 +11140,194 @@
         <v>0</v>
       </c>
       <c r="J39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K39">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L39">
         <v>0</v>
       </c>
       <c r="M39">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N39">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O39">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P39">
-        <v>6</v>
-      </c>
-      <c r="Q39">
-        <v>7</v>
-      </c>
-      <c r="R39">
-        <v>10</v>
-      </c>
-      <c r="S39">
-        <v>5</v>
-      </c>
-      <c r="T39">
-        <v>24</v>
-      </c>
-      <c r="U39">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
+        <v>43516</v>
+      </c>
+      <c r="B40" t="s">
+        <v>237</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>9</v>
+      </c>
+      <c r="G40">
+        <f>R40+T40</f>
+        <v>32</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>4</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>31</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>8</v>
+      </c>
+      <c r="N40">
+        <v>5</v>
+      </c>
+      <c r="O40">
+        <v>4</v>
+      </c>
+      <c r="P40">
+        <v>7</v>
+      </c>
+      <c r="Q40">
+        <v>5</v>
+      </c>
+      <c r="R40">
+        <v>13</v>
+      </c>
+      <c r="S40">
+        <v>5</v>
+      </c>
+      <c r="T40">
+        <v>19</v>
+      </c>
+      <c r="U40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
         <v>43513</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
+        <v>212</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>5</v>
+      </c>
+      <c r="G41">
+        <f t="shared" ref="G41:G66" si="2">R41+T41</f>
+        <v>34</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>4</v>
+      </c>
+      <c r="K41">
+        <v>32</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>9</v>
+      </c>
+      <c r="N41">
+        <v>5</v>
+      </c>
+      <c r="O41">
+        <v>4</v>
+      </c>
+      <c r="P41">
+        <v>6</v>
+      </c>
+      <c r="Q41">
+        <v>7</v>
+      </c>
+      <c r="R41">
+        <v>10</v>
+      </c>
+      <c r="S41">
+        <v>5</v>
+      </c>
+      <c r="T41">
+        <v>24</v>
+      </c>
+      <c r="U41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>43513</v>
+      </c>
+      <c r="B42" t="s">
         <v>213</v>
       </c>
-      <c r="C40">
-        <v>7</v>
-      </c>
-      <c r="D40">
-        <v>5</v>
-      </c>
-      <c r="E40">
-        <v>5</v>
-      </c>
-      <c r="F40">
-        <v>10</v>
-      </c>
-      <c r="G40">
+      <c r="C42">
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>10</v>
+      </c>
+      <c r="G42">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H40">
-        <v>5</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>4</v>
-      </c>
-      <c r="K40">
-        <v>30</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>7</v>
-      </c>
-      <c r="N40">
-        <v>4</v>
-      </c>
-      <c r="O40">
-        <v>6</v>
-      </c>
-      <c r="P40">
-        <v>7</v>
-      </c>
-      <c r="Q40">
-        <v>5</v>
-      </c>
-      <c r="R40">
-        <v>12</v>
-      </c>
-      <c r="S40">
-        <v>4</v>
-      </c>
-      <c r="T40">
-        <v>18</v>
-      </c>
-      <c r="U40">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>43512</v>
-      </c>
-      <c r="B41" t="s">
-        <v>214</v>
-      </c>
-      <c r="C41">
-        <v>6</v>
-      </c>
-      <c r="D41">
-        <v>6</v>
-      </c>
-      <c r="E41">
-        <v>5</v>
-      </c>
-      <c r="F41">
-        <v>10</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="H41">
-        <v>4</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>5</v>
-      </c>
-      <c r="K41">
-        <v>30</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>8</v>
-      </c>
-      <c r="N41">
-        <v>5</v>
-      </c>
-      <c r="O41">
-        <v>5</v>
-      </c>
-      <c r="P41">
-        <v>6</v>
-      </c>
-      <c r="Q41">
-        <v>6</v>
-      </c>
-      <c r="R41">
-        <v>10</v>
-      </c>
-      <c r="S41">
-        <v>5</v>
-      </c>
-      <c r="T41">
-        <v>20</v>
-      </c>
-      <c r="U41">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>43509</v>
-      </c>
-      <c r="B42" t="s">
-        <v>215</v>
-      </c>
-      <c r="C42">
-        <v>6</v>
-      </c>
-      <c r="D42">
-        <v>6</v>
-      </c>
-      <c r="E42">
-        <v>4</v>
-      </c>
-      <c r="F42">
-        <v>11</v>
-      </c>
-      <c r="G42">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
       <c r="H42">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I42">
         <v>0</v>
       </c>
       <c r="J42">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K42">
         <v>30</v>
@@ -11357,64 +11336,64 @@
         <v>0</v>
       </c>
       <c r="M42">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N42">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P42">
         <v>7</v>
       </c>
       <c r="Q42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R42">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S42">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T42">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="U42">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>43508</v>
+        <v>43512</v>
       </c>
       <c r="B43" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D43">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E43">
         <v>5</v>
       </c>
       <c r="F43">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G43">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="H43">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K43">
         <v>30</v>
@@ -11423,79 +11402,79 @@
         <v>0</v>
       </c>
       <c r="M43">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q43">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R43">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T43">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U43">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>43508</v>
+        <v>43509</v>
       </c>
       <c r="B44" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D44">
         <v>6</v>
       </c>
       <c r="E44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G44">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I44">
         <v>0</v>
       </c>
       <c r="J44">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K44">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L44">
         <v>0</v>
       </c>
       <c r="M44">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N44">
         <v>0</v>
       </c>
       <c r="O44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P44">
         <v>7</v>
@@ -11510,18 +11489,18 @@
         <v>0</v>
       </c>
       <c r="T44">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U44">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>43504</v>
+        <v>43508</v>
       </c>
       <c r="B45" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C45">
         <v>7</v>
@@ -11533,32 +11512,32 @@
         <v>5</v>
       </c>
       <c r="F45">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G45">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K45">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L45">
         <v>0</v>
       </c>
       <c r="M45">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N45">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O45">
         <v>6</v>
@@ -11573,10 +11552,10 @@
         <v>11</v>
       </c>
       <c r="S45">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T45">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="U45">
         <v>7</v>
@@ -11584,26 +11563,26 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>43503</v>
+        <v>43508</v>
       </c>
       <c r="B46" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="C46">
         <v>7</v>
       </c>
       <c r="D46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E46">
         <v>5</v>
       </c>
       <c r="F46">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G46">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H46">
         <v>5</v>
@@ -11612,7 +11591,7 @@
         <v>0</v>
       </c>
       <c r="J46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K46">
         <v>32</v>
@@ -11633,7 +11612,7 @@
         <v>7</v>
       </c>
       <c r="Q46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R46">
         <v>11</v>
@@ -11642,7 +11621,7 @@
         <v>0</v>
       </c>
       <c r="T46">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U46">
         <v>7</v>
@@ -11650,35 +11629,35 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>43503</v>
+        <v>43504</v>
       </c>
       <c r="B47" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D47">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F47">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G47">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="H47">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I47">
         <v>0</v>
       </c>
       <c r="J47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K47">
         <v>32</v>
@@ -11687,31 +11666,31 @@
         <v>0</v>
       </c>
       <c r="M47">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O47">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P47">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q47">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R47">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T47">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U47">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
@@ -11719,23 +11698,23 @@
         <v>43503</v>
       </c>
       <c r="B48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D48">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E48">
         <v>5</v>
       </c>
       <c r="F48">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G48">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H48">
         <v>5</v>
@@ -11744,40 +11723,40 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K48">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L48">
         <v>0</v>
       </c>
       <c r="M48">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N48">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O48">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P48">
         <v>7</v>
       </c>
       <c r="Q48">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R48">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S48">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T48">
         <v>22</v>
       </c>
       <c r="U48">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
@@ -11785,125 +11764,125 @@
         <v>43503</v>
       </c>
       <c r="B49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D49">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E49">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F49">
         <v>5</v>
       </c>
       <c r="G49">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I49">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K49">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L49">
         <v>0</v>
       </c>
       <c r="M49">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N49">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P49">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q49">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="R49">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="S49">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T49">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="U49">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>43502</v>
+        <v>43503</v>
       </c>
       <c r="B50" t="s">
-        <v>221</v>
+        <v>154</v>
       </c>
       <c r="C50">
         <v>6</v>
       </c>
       <c r="D50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E50">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50">
         <v>5</v>
       </c>
       <c r="G50">
         <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="H50">
+        <v>5</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
         <v>34</v>
       </c>
-      <c r="H50">
-        <v>5</v>
-      </c>
-      <c r="I50">
-        <v>4</v>
-      </c>
-      <c r="J50">
-        <v>5</v>
-      </c>
-      <c r="K50">
-        <v>30</v>
-      </c>
       <c r="L50">
         <v>0</v>
       </c>
       <c r="M50">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N50">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R50">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S50">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T50">
         <v>22</v>
@@ -11914,38 +11893,38 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>43502</v>
+        <v>43503</v>
       </c>
       <c r="B51" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C51">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E51">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F51">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G51">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H51">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J51">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K51">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -11954,52 +11933,52 @@
         <v>7</v>
       </c>
       <c r="N51">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O51">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P51">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q51">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="R51">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="S51">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T51">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U51">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>43500</v>
+        <v>43502</v>
       </c>
       <c r="B52" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C52">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D52">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F52">
         <v>5</v>
       </c>
       <c r="G52">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H52">
         <v>5</v>
@@ -12017,10 +11996,10 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N52">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O52">
         <v>5</v>
@@ -12029,99 +12008,99 @@
         <v>6</v>
       </c>
       <c r="Q52">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R52">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S52">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T52">
         <v>22</v>
       </c>
       <c r="U52">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>43497</v>
+        <v>43502</v>
       </c>
       <c r="B53" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C53">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D53">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53">
         <v>6</v>
       </c>
       <c r="G53">
         <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H53">
+        <v>4</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>5</v>
+      </c>
+      <c r="K53">
         <v>32</v>
       </c>
-      <c r="H53">
-        <v>5</v>
-      </c>
-      <c r="I53">
-        <v>4</v>
-      </c>
-      <c r="J53">
-        <v>5</v>
-      </c>
-      <c r="K53">
-        <v>31</v>
-      </c>
       <c r="L53">
         <v>0</v>
       </c>
       <c r="M53">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N53">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O53">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P53">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q53">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R53">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S53">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T53">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="U53">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>43496</v>
+        <v>43500</v>
       </c>
       <c r="B54" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D54">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -12131,7 +12110,7 @@
       </c>
       <c r="G54">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H54">
         <v>5</v>
@@ -12140,76 +12119,76 @@
         <v>4</v>
       </c>
       <c r="J54">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K54">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L54">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M54">
         <v>7</v>
       </c>
       <c r="N54">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O54">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P54">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q54">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R54">
         <v>9</v>
       </c>
       <c r="S54">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T54">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="U54">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>43495</v>
+        <v>43497</v>
       </c>
       <c r="B55" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C55">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D55">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F55">
         <v>6</v>
       </c>
       <c r="G55">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I55">
         <v>4</v>
       </c>
       <c r="J55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K55">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L55">
         <v>0</v>
@@ -12221,49 +12200,49 @@
         <v>4</v>
       </c>
       <c r="O55">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q55">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R55">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S55">
         <v>4</v>
       </c>
       <c r="T55">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="U55">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>43495</v>
+        <v>43496</v>
       </c>
       <c r="B56" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C56">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E56">
         <v>4</v>
       </c>
       <c r="F56">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G56">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H56">
         <v>5</v>
@@ -12272,40 +12251,40 @@
         <v>4</v>
       </c>
       <c r="J56">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K56">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M56">
         <v>7</v>
       </c>
       <c r="N56">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O56">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P56">
         <v>7</v>
       </c>
       <c r="Q56">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R56">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S56">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T56">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U56">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
@@ -12313,47 +12292,47 @@
         <v>43495</v>
       </c>
       <c r="B57" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C57">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D57">
         <v>6</v>
       </c>
       <c r="E57">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F57">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G57">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H57">
         <v>4</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J57">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K57">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L57">
         <v>0</v>
       </c>
       <c r="M57">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N57">
         <v>4</v>
       </c>
       <c r="O57">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P57">
         <v>6</v>
@@ -12368,10 +12347,10 @@
         <v>4</v>
       </c>
       <c r="T57">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U57">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
@@ -12379,23 +12358,23 @@
         <v>43495</v>
       </c>
       <c r="B58" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C58">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D58">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E58">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G58">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H58">
         <v>5</v>
@@ -12404,10 +12383,10 @@
         <v>4</v>
       </c>
       <c r="J58">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K58">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L58">
         <v>0</v>
@@ -12419,33 +12398,33 @@
         <v>4</v>
       </c>
       <c r="O58">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P58">
         <v>7</v>
       </c>
       <c r="Q58">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R58">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S58">
         <v>4</v>
       </c>
       <c r="T58">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="U58">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>43489</v>
+        <v>43495</v>
       </c>
       <c r="B59" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C59">
         <v>6</v>
@@ -12457,17 +12436,17 @@
         <v>6</v>
       </c>
       <c r="F59">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G59">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H59">
         <v>4</v>
       </c>
       <c r="I59">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J59">
         <v>5</v>
@@ -12485,7 +12464,7 @@
         <v>4</v>
       </c>
       <c r="O59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P59">
         <v>6</v>
@@ -12494,13 +12473,13 @@
         <v>6</v>
       </c>
       <c r="R59">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S59">
         <v>4</v>
       </c>
       <c r="T59">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="U59">
         <v>6</v>
@@ -12508,32 +12487,32 @@
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>43487</v>
+        <v>43495</v>
       </c>
       <c r="B60" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C60">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D60">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E60">
         <v>5</v>
       </c>
       <c r="F60">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G60">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H60">
         <v>5</v>
       </c>
       <c r="I60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J60">
         <v>5</v>
@@ -12551,64 +12530,67 @@
         <v>4</v>
       </c>
       <c r="O60">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P60">
         <v>7</v>
       </c>
       <c r="Q60">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R60">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S60">
         <v>4</v>
       </c>
       <c r="T60">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="U60">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>43482</v>
+        <v>43489</v>
       </c>
       <c r="B61" t="s">
-        <v>232</v>
+        <v>230</v>
+      </c>
+      <c r="C61">
+        <v>6</v>
       </c>
       <c r="D61">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E61">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F61">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G61">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H61">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I61">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J61">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K61">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L61">
         <v>0</v>
       </c>
       <c r="M61">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N61">
         <v>4</v>
@@ -12617,13 +12599,13 @@
         <v>5</v>
       </c>
       <c r="P61">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q61">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="R61">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S61">
         <v>4</v>
@@ -12631,73 +12613,82 @@
       <c r="T61">
         <v>15</v>
       </c>
+      <c r="U61">
+        <v>6</v>
+      </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>43482</v>
+        <v>43487</v>
       </c>
       <c r="B62" t="s">
-        <v>233</v>
+        <v>231</v>
+      </c>
+      <c r="C62">
+        <v>6</v>
       </c>
       <c r="D62">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E62">
         <v>5</v>
       </c>
       <c r="F62">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G62">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H62">
         <v>5</v>
       </c>
       <c r="I62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K62">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L62">
         <v>0</v>
       </c>
       <c r="M62">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N62">
         <v>4</v>
       </c>
       <c r="O62">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P62">
         <v>7</v>
       </c>
       <c r="Q62">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R62">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="S62">
         <v>4</v>
       </c>
       <c r="T62">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="U62">
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>43481</v>
+        <v>43482</v>
       </c>
       <c r="B63" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D63">
         <v>12</v>
@@ -12706,26 +12697,29 @@
         <v>5</v>
       </c>
       <c r="F63">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G63">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H63">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I63">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J63">
         <v>4</v>
       </c>
       <c r="K63">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
       </c>
       <c r="M63">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N63">
         <v>4</v>
@@ -12734,84 +12728,201 @@
         <v>5</v>
       </c>
       <c r="P63">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q63">
         <v>12</v>
       </c>
       <c r="R63">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="S63">
         <v>4</v>
       </c>
       <c r="T63">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>43481</v>
+        <v>43482</v>
       </c>
       <c r="B64" t="s">
-        <v>235</v>
-      </c>
-      <c r="C64">
-        <v>6</v>
+        <v>233</v>
       </c>
       <c r="D64">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E64">
         <v>5</v>
       </c>
       <c r="F64">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G64">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I64">
         <v>4</v>
       </c>
       <c r="J64">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K64">
+        <v>33</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>9</v>
+      </c>
+      <c r="N64">
+        <v>4</v>
+      </c>
+      <c r="O64">
+        <v>4</v>
+      </c>
+      <c r="P64">
+        <v>7</v>
+      </c>
+      <c r="Q64">
+        <v>10</v>
+      </c>
+      <c r="R64">
+        <v>15</v>
+      </c>
+      <c r="S64">
+        <v>4</v>
+      </c>
+      <c r="T64">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>43481</v>
+      </c>
+      <c r="B65" t="s">
+        <v>234</v>
+      </c>
+      <c r="D65">
+        <v>12</v>
+      </c>
+      <c r="E65">
+        <v>5</v>
+      </c>
+      <c r="F65">
+        <v>7</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="H65">
+        <v>6</v>
+      </c>
+      <c r="I65">
+        <v>6</v>
+      </c>
+      <c r="J65">
+        <v>4</v>
+      </c>
+      <c r="K65">
+        <v>31</v>
+      </c>
+      <c r="M65">
+        <v>7</v>
+      </c>
+      <c r="N65">
+        <v>4</v>
+      </c>
+      <c r="O65">
+        <v>5</v>
+      </c>
+      <c r="P65">
+        <v>6</v>
+      </c>
+      <c r="Q65">
+        <v>12</v>
+      </c>
+      <c r="R65">
+        <v>10</v>
+      </c>
+      <c r="S65">
+        <v>4</v>
+      </c>
+      <c r="T65">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>43481</v>
+      </c>
+      <c r="B66" t="s">
+        <v>235</v>
+      </c>
+      <c r="C66">
+        <v>6</v>
+      </c>
+      <c r="D66">
+        <v>6</v>
+      </c>
+      <c r="E66">
+        <v>5</v>
+      </c>
+      <c r="F66">
+        <v>9</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="H66">
+        <v>4</v>
+      </c>
+      <c r="I66">
+        <v>4</v>
+      </c>
+      <c r="J66">
+        <v>6</v>
+      </c>
+      <c r="K66">
         <v>32</v>
       </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
-      <c r="M64">
-        <v>8</v>
-      </c>
-      <c r="N64">
-        <v>0</v>
-      </c>
-      <c r="O64">
-        <v>6</v>
-      </c>
-      <c r="P64">
-        <v>7</v>
-      </c>
-      <c r="Q64">
-        <v>6</v>
-      </c>
-      <c r="R64">
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>8</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>6</v>
+      </c>
+      <c r="P66">
+        <v>7</v>
+      </c>
+      <c r="Q66">
+        <v>6</v>
+      </c>
+      <c r="R66">
         <v>14</v>
       </c>
-      <c r="S64">
-        <v>0</v>
-      </c>
-      <c r="T64">
+      <c r="S66">
+        <v>0</v>
+      </c>
+      <c r="T66">
         <v>13</v>
       </c>
-      <c r="U64">
+      <c r="U66">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated polls 28 Mar 2019
</commit_message>
<xml_diff>
--- a/Data/polls.xlsx
+++ b/Data/polls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mac Tan\Desktop\Stuff\Elections\2019\Israel-2019\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E274BEFC-0C73-4EC9-80A2-33B74B7573C3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F217713B-E02E-48D3-9F8C-CE56C161150E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="3" xr2:uid="{0DE1B94D-B05B-4FF7-9BF3-1803C0C1CFBD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="277">
   <si>
     <t>Channel 2[5]</t>
   </si>
@@ -860,6 +860,12 @@
   </si>
   <si>
     <t>Midgam/Army Radio[4]</t>
+  </si>
+  <si>
+    <t>Panels Politics/Walla![10]</t>
+  </si>
+  <si>
+    <t>Channel 13[8]</t>
   </si>
 </sst>
 </file>
@@ -9037,10 +9043,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CC49F9-512D-4648-8DF6-8D5ABA179EFE}">
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:V68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -9115,16 +9121,16 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>43550</v>
+        <v>43552</v>
       </c>
       <c r="B2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -9136,82 +9142,82 @@
         <v>30</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>4</v>
       </c>
       <c r="J2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M2">
         <v>5</v>
       </c>
       <c r="N2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P2">
         <v>7</v>
       </c>
       <c r="V2">
-        <f t="shared" ref="V2:V8" si="0">SUM(C2:P2)</f>
+        <f t="shared" ref="V2:V10" si="0">SUM(C2:P2)</f>
         <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>43550</v>
+        <v>43551</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>30</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K3">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P3">
         <v>7</v>
@@ -9223,28 +9229,28 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>43548</v>
+        <v>43550</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I4">
         <v>4</v>
@@ -9277,28 +9283,28 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>43548</v>
+        <v>43550</v>
       </c>
       <c r="B5" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="C5">
         <v>7</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>5</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G5">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -9313,16 +9319,16 @@
         <v>6</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V5">
         <f t="shared" si="0"/>
@@ -9331,37 +9337,37 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>43546</v>
+        <v>43548</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K6">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -9370,10 +9376,10 @@
         <v>5</v>
       </c>
       <c r="N6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P6">
         <v>7</v>
@@ -9385,37 +9391,37 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>43546</v>
+        <v>43548</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L7">
         <v>6</v>
@@ -9424,10 +9430,10 @@
         <v>5</v>
       </c>
       <c r="N7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P7">
         <v>6</v>
@@ -9442,46 +9448,46 @@
         <v>43546</v>
       </c>
       <c r="B8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <v>30</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K8">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L8">
         <v>4</v>
       </c>
       <c r="M8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N8">
         <v>6</v>
       </c>
       <c r="O8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P8">
         <v>7</v>
@@ -9493,67 +9499,67 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>43544</v>
+        <v>43546</v>
       </c>
       <c r="B9" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H9">
         <v>4</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J9">
         <v>4</v>
       </c>
       <c r="K9">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V9">
-        <f>SUM(C9:P9)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>43544</v>
+        <v>43546</v>
       </c>
       <c r="B10" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -9562,10 +9568,10 @@
         <v>5</v>
       </c>
       <c r="F10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10">
         <v>5</v>
@@ -9574,13 +9580,13 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K10">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M10">
         <v>6</v>
@@ -9589,37 +9595,37 @@
         <v>6</v>
       </c>
       <c r="O10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P10">
         <v>7</v>
       </c>
       <c r="V10">
-        <f t="shared" ref="V10:V39" si="1">SUM(C10:P10)</f>
-        <v>119</v>
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>43543</v>
+        <v>43544</v>
       </c>
       <c r="B11" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G11">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H11">
         <v>4</v>
@@ -9628,10 +9634,10 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K11">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="L11">
         <v>4</v>
@@ -9640,55 +9646,55 @@
         <v>6</v>
       </c>
       <c r="N11">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V11">
-        <f t="shared" si="1"/>
+        <f>SUM(C11:P11)</f>
         <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>43541</v>
+        <v>43544</v>
       </c>
       <c r="B12" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <v>9</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M12">
         <v>6</v>
@@ -9697,40 +9703,40 @@
         <v>6</v>
       </c>
       <c r="O12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V12">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <f t="shared" ref="V12:V41" si="1">SUM(C12:P12)</f>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>43538</v>
+        <v>43543</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G13">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -9739,10 +9745,10 @@
         <v>5</v>
       </c>
       <c r="K13">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M13">
         <v>6</v>
@@ -9751,10 +9757,10 @@
         <v>7</v>
       </c>
       <c r="O13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V13">
         <f t="shared" si="1"/>
@@ -9763,52 +9769,52 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>43538</v>
+        <v>43541</v>
       </c>
       <c r="B14" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14">
+        <v>30</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
         <v>31</v>
       </c>
-      <c r="H14">
-        <v>4</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>4</v>
-      </c>
-      <c r="K14">
-        <v>28</v>
-      </c>
       <c r="L14">
         <v>4</v>
       </c>
       <c r="M14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O14">
         <v>6</v>
       </c>
       <c r="P14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V14">
         <f t="shared" si="1"/>
@@ -9817,49 +9823,49 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>43537</v>
+        <v>43538</v>
       </c>
       <c r="B15" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="C15">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F15">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G15">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K15">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N15">
         <v>7</v>
       </c>
       <c r="O15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P15">
         <v>7</v>
@@ -9871,22 +9877,22 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>43535</v>
+        <v>43538</v>
       </c>
       <c r="B16" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C16">
         <v>7</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G16">
         <v>31</v>
@@ -9907,16 +9913,16 @@
         <v>4</v>
       </c>
       <c r="M16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N16">
         <v>7</v>
       </c>
       <c r="O16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V16">
         <f t="shared" si="1"/>
@@ -9925,46 +9931,46 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>43532</v>
+        <v>43537</v>
       </c>
       <c r="B17" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C17">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F17">
         <v>10</v>
       </c>
       <c r="G17">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O17">
         <v>6</v>
@@ -9979,22 +9985,22 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>43531</v>
+        <v>43535</v>
       </c>
       <c r="B18" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G18">
         <v>31</v>
@@ -10006,7 +10012,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K18">
         <v>28</v>
@@ -10015,16 +10021,16 @@
         <v>4</v>
       </c>
       <c r="M18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O18">
         <v>5</v>
       </c>
       <c r="P18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V18">
         <f t="shared" si="1"/>
@@ -10033,22 +10039,22 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>43531</v>
+        <v>43532</v>
       </c>
       <c r="B19" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F19">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G19">
         <v>33</v>
@@ -10060,25 +10066,25 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K19">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L19">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V19">
         <f t="shared" si="1"/>
@@ -10087,10 +10093,10 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>43529</v>
+        <v>43531</v>
       </c>
       <c r="B20" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -10099,16 +10105,16 @@
         <v>4</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -10117,16 +10123,16 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L20">
         <v>4</v>
       </c>
       <c r="M20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N20">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O20">
         <v>5</v>
@@ -10141,52 +10147,52 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>43529</v>
+        <v>43531</v>
       </c>
       <c r="B21" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C21">
         <v>9</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G21">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H21">
         <v>4</v>
       </c>
       <c r="I21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K21">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="V21">
         <f t="shared" si="1"/>
@@ -10198,7 +10204,7 @@
         <v>43529</v>
       </c>
       <c r="B22" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C22">
         <v>8</v>
@@ -10207,13 +10213,13 @@
         <v>4</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F22">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G22">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H22">
         <v>5</v>
@@ -10228,23 +10234,23 @@
         <v>30</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M22">
         <v>5</v>
       </c>
       <c r="N22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P22">
         <v>7</v>
       </c>
       <c r="V22">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -10252,34 +10258,34 @@
         <v>43529</v>
       </c>
       <c r="B23" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C23">
         <v>9</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G23">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K23">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -10288,13 +10294,13 @@
         <v>6</v>
       </c>
       <c r="N23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V23">
         <f t="shared" si="1"/>
@@ -10303,25 +10309,25 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>43527</v>
+        <v>43529</v>
       </c>
       <c r="B24" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G24">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H24">
         <v>5</v>
@@ -10339,10 +10345,10 @@
         <v>0</v>
       </c>
       <c r="M24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O24">
         <v>4</v>
@@ -10352,33 +10358,33 @@
       </c>
       <c r="V24">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>43525</v>
+        <v>43529</v>
       </c>
       <c r="B25" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C25">
         <v>9</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>6</v>
       </c>
       <c r="F25">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G25">
         <v>36</v>
       </c>
       <c r="H25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -10387,19 +10393,19 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N25">
         <v>7</v>
       </c>
       <c r="O25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P25">
         <v>7</v>
@@ -10411,25 +10417,25 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>43525</v>
+        <v>43527</v>
       </c>
       <c r="B26" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C26">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>6</v>
       </c>
       <c r="F26">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G26">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H26">
         <v>5</v>
@@ -10441,19 +10447,19 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N26">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O26">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P26">
         <v>7</v>
@@ -10468,25 +10474,25 @@
         <v>43525</v>
       </c>
       <c r="B27" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27">
         <v>6</v>
       </c>
       <c r="F27">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G27">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -10495,49 +10501,49 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N27">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O27">
         <v>6</v>
       </c>
       <c r="P27">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V27">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>43524</v>
+        <v>43525</v>
       </c>
       <c r="B28" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C28">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F28">
         <v>6</v>
       </c>
       <c r="G28">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H28">
         <v>5</v>
@@ -10546,7 +10552,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K28">
         <v>29</v>
@@ -10555,13 +10561,13 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N28">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P28">
         <v>7</v>
@@ -10573,28 +10579,28 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>43524</v>
+        <v>43525</v>
       </c>
       <c r="B29" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C29">
         <v>7</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E29">
         <v>6</v>
       </c>
       <c r="F29">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G29">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -10603,7 +10609,7 @@
         <v>0</v>
       </c>
       <c r="K29">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -10612,7 +10618,7 @@
         <v>8</v>
       </c>
       <c r="N29">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O29">
         <v>6</v>
@@ -10622,33 +10628,33 @@
       </c>
       <c r="V29">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>43523</v>
+        <v>43524</v>
       </c>
       <c r="B30" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C30">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F30">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G30">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -10663,13 +10669,13 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N30">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P30">
         <v>7</v>
@@ -10681,10 +10687,10 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>43520</v>
+        <v>43524</v>
       </c>
       <c r="B31" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C31">
         <v>7</v>
@@ -10693,16 +10699,16 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G31">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -10711,22 +10717,22 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L31">
         <v>0</v>
       </c>
       <c r="M31">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N31">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O31">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P31">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V31">
         <f t="shared" si="1"/>
@@ -10735,25 +10741,25 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>43520</v>
+        <v>43523</v>
       </c>
       <c r="B32" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C32">
         <v>7</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E32">
         <v>4</v>
       </c>
       <c r="F32">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G32">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H32">
         <v>4</v>
@@ -10771,13 +10777,13 @@
         <v>0</v>
       </c>
       <c r="M32">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N32">
         <v>5</v>
       </c>
       <c r="O32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P32">
         <v>7</v>
@@ -10789,67 +10795,67 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>43518</v>
+        <v>43520</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C33">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D33">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F33">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G33">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H33">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K33">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
       <c r="M33">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O33">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P33">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V33">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>43517</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>242</v>
+        <v>43520</v>
+      </c>
+      <c r="B34" t="s">
+        <v>250</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34">
         <v>5</v>
@@ -10858,7 +10864,7 @@
         <v>4</v>
       </c>
       <c r="F34">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G34">
         <v>35</v>
@@ -10879,10 +10885,10 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O34">
         <v>5</v>
@@ -10897,25 +10903,25 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>43517</v>
+        <v>43518</v>
       </c>
       <c r="B35" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C35">
         <v>6</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F35">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G35">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H35">
         <v>4</v>
@@ -10927,7 +10933,7 @@
         <v>4</v>
       </c>
       <c r="K35">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -10936,31 +10942,31 @@
         <v>6</v>
       </c>
       <c r="N35">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P35">
         <v>6</v>
       </c>
       <c r="V35">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>43517</v>
       </c>
-      <c r="B36" t="s">
-        <v>244</v>
+      <c r="B36" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="C36">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -10972,16 +10978,16 @@
         <v>35</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
       <c r="J36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K36">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -11008,13 +11014,13 @@
         <v>43517</v>
       </c>
       <c r="B37" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C37">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -11023,31 +11029,31 @@
         <v>8</v>
       </c>
       <c r="G37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I37">
         <v>0</v>
       </c>
       <c r="J37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K37">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L37">
         <v>0</v>
       </c>
       <c r="M37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P37">
         <v>6</v>
@@ -11062,43 +11068,43 @@
         <v>43517</v>
       </c>
       <c r="B38" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C38">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>4</v>
       </c>
       <c r="F38">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G38">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H38">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I38">
         <v>0</v>
       </c>
       <c r="J38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K38">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N38">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O38">
         <v>5</v>
@@ -11116,25 +11122,25 @@
         <v>43517</v>
       </c>
       <c r="B39" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C39">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D39">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>4</v>
       </c>
       <c r="F39">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G39">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -11143,22 +11149,22 @@
         <v>5</v>
       </c>
       <c r="K39">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L39">
         <v>0</v>
       </c>
       <c r="M39">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N39">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O39">
         <v>6</v>
       </c>
       <c r="P39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V39">
         <f t="shared" si="1"/>
@@ -11167,82 +11173,70 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="B40" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="C40">
         <v>6</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G40">
-        <f>R40+T40</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H40">
         <v>4</v>
       </c>
       <c r="I40">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K40">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L40">
         <v>0</v>
       </c>
       <c r="M40">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P40">
         <v>7</v>
       </c>
-      <c r="Q40">
-        <v>5</v>
-      </c>
-      <c r="R40">
-        <v>13</v>
-      </c>
-      <c r="S40">
-        <v>5</v>
-      </c>
-      <c r="T40">
-        <v>19</v>
-      </c>
-      <c r="U40">
-        <v>6</v>
+      <c r="V40">
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>43513</v>
+        <v>43517</v>
       </c>
       <c r="B41" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D41">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -11251,8 +11245,7 @@
         <v>5</v>
       </c>
       <c r="G41">
-        <f t="shared" ref="G41:G66" si="2">R41+T41</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H41">
         <v>4</v>
@@ -11261,205 +11254,194 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K41">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L41">
         <v>0</v>
       </c>
       <c r="M41">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N41">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P41">
-        <v>6</v>
-      </c>
-      <c r="Q41">
-        <v>7</v>
-      </c>
-      <c r="R41">
-        <v>10</v>
-      </c>
-      <c r="S41">
-        <v>5</v>
-      </c>
-      <c r="T41">
-        <v>24</v>
-      </c>
-      <c r="U41">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
+        <v>43516</v>
+      </c>
+      <c r="B42" t="s">
+        <v>237</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>9</v>
+      </c>
+      <c r="G42">
+        <f>R42+T42</f>
+        <v>32</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>4</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>31</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>8</v>
+      </c>
+      <c r="N42">
+        <v>5</v>
+      </c>
+      <c r="O42">
+        <v>4</v>
+      </c>
+      <c r="P42">
+        <v>7</v>
+      </c>
+      <c r="Q42">
+        <v>5</v>
+      </c>
+      <c r="R42">
+        <v>13</v>
+      </c>
+      <c r="S42">
+        <v>5</v>
+      </c>
+      <c r="T42">
+        <v>19</v>
+      </c>
+      <c r="U42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
         <v>43513</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
+        <v>212</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43">
+        <f t="shared" ref="G43:G68" si="2">R43+T43</f>
+        <v>34</v>
+      </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>4</v>
+      </c>
+      <c r="K43">
+        <v>32</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>9</v>
+      </c>
+      <c r="N43">
+        <v>5</v>
+      </c>
+      <c r="O43">
+        <v>4</v>
+      </c>
+      <c r="P43">
+        <v>6</v>
+      </c>
+      <c r="Q43">
+        <v>7</v>
+      </c>
+      <c r="R43">
+        <v>10</v>
+      </c>
+      <c r="S43">
+        <v>5</v>
+      </c>
+      <c r="T43">
+        <v>24</v>
+      </c>
+      <c r="U43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>43513</v>
+      </c>
+      <c r="B44" t="s">
         <v>213</v>
       </c>
-      <c r="C42">
-        <v>7</v>
-      </c>
-      <c r="D42">
-        <v>5</v>
-      </c>
-      <c r="E42">
-        <v>5</v>
-      </c>
-      <c r="F42">
-        <v>10</v>
-      </c>
-      <c r="G42">
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>10</v>
+      </c>
+      <c r="G44">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H42">
-        <v>5</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>4</v>
-      </c>
-      <c r="K42">
-        <v>30</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>7</v>
-      </c>
-      <c r="N42">
-        <v>4</v>
-      </c>
-      <c r="O42">
-        <v>6</v>
-      </c>
-      <c r="P42">
-        <v>7</v>
-      </c>
-      <c r="Q42">
-        <v>5</v>
-      </c>
-      <c r="R42">
-        <v>12</v>
-      </c>
-      <c r="S42">
-        <v>4</v>
-      </c>
-      <c r="T42">
-        <v>18</v>
-      </c>
-      <c r="U42">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>43512</v>
-      </c>
-      <c r="B43" t="s">
-        <v>214</v>
-      </c>
-      <c r="C43">
-        <v>6</v>
-      </c>
-      <c r="D43">
-        <v>6</v>
-      </c>
-      <c r="E43">
-        <v>5</v>
-      </c>
-      <c r="F43">
-        <v>10</v>
-      </c>
-      <c r="G43">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="H43">
-        <v>4</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>5</v>
-      </c>
-      <c r="K43">
-        <v>30</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>8</v>
-      </c>
-      <c r="N43">
-        <v>5</v>
-      </c>
-      <c r="O43">
-        <v>5</v>
-      </c>
-      <c r="P43">
-        <v>6</v>
-      </c>
-      <c r="Q43">
-        <v>6</v>
-      </c>
-      <c r="R43">
-        <v>10</v>
-      </c>
-      <c r="S43">
-        <v>5</v>
-      </c>
-      <c r="T43">
-        <v>20</v>
-      </c>
-      <c r="U43">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>43509</v>
-      </c>
-      <c r="B44" t="s">
-        <v>215</v>
-      </c>
-      <c r="C44">
-        <v>6</v>
-      </c>
-      <c r="D44">
-        <v>6</v>
-      </c>
-      <c r="E44">
-        <v>4</v>
-      </c>
-      <c r="F44">
-        <v>11</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
       <c r="H44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I44">
         <v>0</v>
       </c>
       <c r="J44">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K44">
         <v>30</v>
@@ -11468,64 +11450,64 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N44">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P44">
         <v>7</v>
       </c>
       <c r="Q44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R44">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S44">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T44">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="U44">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>43508</v>
+        <v>43512</v>
       </c>
       <c r="B45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C45">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E45">
         <v>5</v>
       </c>
       <c r="F45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G45">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="H45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I45">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K45">
         <v>30</v>
@@ -11534,79 +11516,79 @@
         <v>0</v>
       </c>
       <c r="M45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P45">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R45">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S45">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T45">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U45">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>43508</v>
+        <v>43509</v>
       </c>
       <c r="B46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C46">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D46">
         <v>6</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G46">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I46">
         <v>0</v>
       </c>
       <c r="J46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K46">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L46">
         <v>0</v>
       </c>
       <c r="M46">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N46">
         <v>0</v>
       </c>
       <c r="O46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P46">
         <v>7</v>
@@ -11621,18 +11603,18 @@
         <v>0</v>
       </c>
       <c r="T46">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U46">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>43504</v>
+        <v>43508</v>
       </c>
       <c r="B47" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C47">
         <v>7</v>
@@ -11644,32 +11626,32 @@
         <v>5</v>
       </c>
       <c r="F47">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G47">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K47">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L47">
         <v>0</v>
       </c>
       <c r="M47">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N47">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O47">
         <v>6</v>
@@ -11684,10 +11666,10 @@
         <v>11</v>
       </c>
       <c r="S47">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T47">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="U47">
         <v>7</v>
@@ -11695,26 +11677,26 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>43503</v>
+        <v>43508</v>
       </c>
       <c r="B48" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="C48">
         <v>7</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E48">
         <v>5</v>
       </c>
       <c r="F48">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G48">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H48">
         <v>5</v>
@@ -11723,7 +11705,7 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K48">
         <v>32</v>
@@ -11744,7 +11726,7 @@
         <v>7</v>
       </c>
       <c r="Q48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R48">
         <v>11</v>
@@ -11753,7 +11735,7 @@
         <v>0</v>
       </c>
       <c r="T48">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U48">
         <v>7</v>
@@ -11761,35 +11743,35 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>43503</v>
+        <v>43504</v>
       </c>
       <c r="B49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C49">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F49">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="H49">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I49">
         <v>0</v>
       </c>
       <c r="J49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K49">
         <v>32</v>
@@ -11798,31 +11780,31 @@
         <v>0</v>
       </c>
       <c r="M49">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P49">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R49">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T49">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U49">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
@@ -11830,23 +11812,23 @@
         <v>43503</v>
       </c>
       <c r="B50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D50">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E50">
         <v>5</v>
       </c>
       <c r="F50">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G50">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H50">
         <v>5</v>
@@ -11855,40 +11837,40 @@
         <v>0</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K50">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L50">
         <v>0</v>
       </c>
       <c r="M50">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N50">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O50">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P50">
         <v>7</v>
       </c>
       <c r="Q50">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R50">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S50">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T50">
         <v>22</v>
       </c>
       <c r="U50">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
@@ -11896,125 +11878,125 @@
         <v>43503</v>
       </c>
       <c r="B51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D51">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E51">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F51">
         <v>5</v>
       </c>
       <c r="G51">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I51">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J51">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K51">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L51">
         <v>0</v>
       </c>
       <c r="M51">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N51">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O51">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P51">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q51">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="R51">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="S51">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T51">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="U51">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>43502</v>
+        <v>43503</v>
       </c>
       <c r="B52" t="s">
-        <v>221</v>
+        <v>154</v>
       </c>
       <c r="C52">
         <v>6</v>
       </c>
       <c r="D52">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E52">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52">
         <v>5</v>
       </c>
       <c r="G52">
         <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="H52">
+        <v>5</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
         <v>34</v>
       </c>
-      <c r="H52">
-        <v>5</v>
-      </c>
-      <c r="I52">
-        <v>4</v>
-      </c>
-      <c r="J52">
-        <v>5</v>
-      </c>
-      <c r="K52">
-        <v>30</v>
-      </c>
       <c r="L52">
         <v>0</v>
       </c>
       <c r="M52">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N52">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O52">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P52">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q52">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R52">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S52">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T52">
         <v>22</v>
@@ -12025,38 +12007,38 @@
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>43502</v>
+        <v>43503</v>
       </c>
       <c r="B53" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C53">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E53">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F53">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G53">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H53">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J53">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K53">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L53">
         <v>0</v>
@@ -12065,52 +12047,52 @@
         <v>7</v>
       </c>
       <c r="N53">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O53">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P53">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q53">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="R53">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="S53">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T53">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U53">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>43500</v>
+        <v>43502</v>
       </c>
       <c r="B54" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D54">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E54">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F54">
         <v>5</v>
       </c>
       <c r="G54">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H54">
         <v>5</v>
@@ -12128,10 +12110,10 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N54">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O54">
         <v>5</v>
@@ -12140,99 +12122,99 @@
         <v>6</v>
       </c>
       <c r="Q54">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R54">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S54">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T54">
         <v>22</v>
       </c>
       <c r="U54">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>43497</v>
+        <v>43502</v>
       </c>
       <c r="B55" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E55">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55">
         <v>6</v>
       </c>
       <c r="G55">
         <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>5</v>
+      </c>
+      <c r="K55">
         <v>32</v>
       </c>
-      <c r="H55">
-        <v>5</v>
-      </c>
-      <c r="I55">
-        <v>4</v>
-      </c>
-      <c r="J55">
-        <v>5</v>
-      </c>
-      <c r="K55">
-        <v>31</v>
-      </c>
       <c r="L55">
         <v>0</v>
       </c>
       <c r="M55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P55">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q55">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R55">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T55">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="U55">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>43496</v>
+        <v>43500</v>
       </c>
       <c r="B56" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D56">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E56">
         <v>4</v>
@@ -12242,7 +12224,7 @@
       </c>
       <c r="G56">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H56">
         <v>5</v>
@@ -12251,76 +12233,76 @@
         <v>4</v>
       </c>
       <c r="J56">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K56">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L56">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M56">
         <v>7</v>
       </c>
       <c r="N56">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O56">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q56">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R56">
         <v>9</v>
       </c>
       <c r="S56">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T56">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="U56">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>43495</v>
+        <v>43497</v>
       </c>
       <c r="B57" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C57">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D57">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E57">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F57">
         <v>6</v>
       </c>
       <c r="G57">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H57">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I57">
         <v>4</v>
       </c>
       <c r="J57">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K57">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L57">
         <v>0</v>
@@ -12332,49 +12314,49 @@
         <v>4</v>
       </c>
       <c r="O57">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P57">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q57">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R57">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S57">
         <v>4</v>
       </c>
       <c r="T57">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="U57">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>43495</v>
+        <v>43496</v>
       </c>
       <c r="B58" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C58">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E58">
         <v>4</v>
       </c>
       <c r="F58">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G58">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H58">
         <v>5</v>
@@ -12383,40 +12365,40 @@
         <v>4</v>
       </c>
       <c r="J58">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K58">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L58">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M58">
         <v>7</v>
       </c>
       <c r="N58">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O58">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P58">
         <v>7</v>
       </c>
       <c r="Q58">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R58">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S58">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T58">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U58">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
@@ -12424,47 +12406,47 @@
         <v>43495</v>
       </c>
       <c r="B59" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C59">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D59">
         <v>6</v>
       </c>
       <c r="E59">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F59">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G59">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H59">
         <v>4</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K59">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L59">
         <v>0</v>
       </c>
       <c r="M59">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N59">
         <v>4</v>
       </c>
       <c r="O59">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P59">
         <v>6</v>
@@ -12479,10 +12461,10 @@
         <v>4</v>
       </c>
       <c r="T59">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U59">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
@@ -12490,23 +12472,23 @@
         <v>43495</v>
       </c>
       <c r="B60" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D60">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G60">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H60">
         <v>5</v>
@@ -12515,10 +12497,10 @@
         <v>4</v>
       </c>
       <c r="J60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K60">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L60">
         <v>0</v>
@@ -12530,33 +12512,33 @@
         <v>4</v>
       </c>
       <c r="O60">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P60">
         <v>7</v>
       </c>
       <c r="Q60">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R60">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S60">
         <v>4</v>
       </c>
       <c r="T60">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="U60">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>43489</v>
+        <v>43495</v>
       </c>
       <c r="B61" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C61">
         <v>6</v>
@@ -12568,17 +12550,17 @@
         <v>6</v>
       </c>
       <c r="F61">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G61">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H61">
         <v>4</v>
       </c>
       <c r="I61">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J61">
         <v>5</v>
@@ -12596,7 +12578,7 @@
         <v>4</v>
       </c>
       <c r="O61">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P61">
         <v>6</v>
@@ -12605,13 +12587,13 @@
         <v>6</v>
       </c>
       <c r="R61">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S61">
         <v>4</v>
       </c>
       <c r="T61">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="U61">
         <v>6</v>
@@ -12619,32 +12601,32 @@
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>43487</v>
+        <v>43495</v>
       </c>
       <c r="B62" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C62">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D62">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E62">
         <v>5</v>
       </c>
       <c r="F62">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G62">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H62">
         <v>5</v>
       </c>
       <c r="I62">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J62">
         <v>5</v>
@@ -12662,64 +12644,67 @@
         <v>4</v>
       </c>
       <c r="O62">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P62">
         <v>7</v>
       </c>
       <c r="Q62">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R62">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S62">
         <v>4</v>
       </c>
       <c r="T62">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="U62">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>43482</v>
+        <v>43489</v>
       </c>
       <c r="B63" t="s">
-        <v>232</v>
+        <v>230</v>
+      </c>
+      <c r="C63">
+        <v>6</v>
       </c>
       <c r="D63">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E63">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F63">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G63">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H63">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I63">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J63">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K63">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L63">
         <v>0</v>
       </c>
       <c r="M63">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N63">
         <v>4</v>
@@ -12728,13 +12713,13 @@
         <v>5</v>
       </c>
       <c r="P63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q63">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="R63">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S63">
         <v>4</v>
@@ -12742,73 +12727,82 @@
       <c r="T63">
         <v>15</v>
       </c>
+      <c r="U63">
+        <v>6</v>
+      </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>43482</v>
+        <v>43487</v>
       </c>
       <c r="B64" t="s">
-        <v>233</v>
+        <v>231</v>
+      </c>
+      <c r="C64">
+        <v>6</v>
       </c>
       <c r="D64">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E64">
         <v>5</v>
       </c>
       <c r="F64">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G64">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H64">
         <v>5</v>
       </c>
       <c r="I64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K64">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L64">
         <v>0</v>
       </c>
       <c r="M64">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N64">
         <v>4</v>
       </c>
       <c r="O64">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P64">
         <v>7</v>
       </c>
       <c r="Q64">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R64">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="S64">
         <v>4</v>
       </c>
       <c r="T64">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="U64">
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>43481</v>
+        <v>43482</v>
       </c>
       <c r="B65" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D65">
         <v>12</v>
@@ -12817,26 +12811,29 @@
         <v>5</v>
       </c>
       <c r="F65">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G65">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H65">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I65">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J65">
         <v>4</v>
       </c>
       <c r="K65">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
       </c>
       <c r="M65">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N65">
         <v>4</v>
@@ -12845,84 +12842,201 @@
         <v>5</v>
       </c>
       <c r="P65">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q65">
         <v>12</v>
       </c>
       <c r="R65">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="S65">
         <v>4</v>
       </c>
       <c r="T65">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>43481</v>
+        <v>43482</v>
       </c>
       <c r="B66" t="s">
-        <v>235</v>
-      </c>
-      <c r="C66">
-        <v>6</v>
+        <v>233</v>
       </c>
       <c r="D66">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E66">
         <v>5</v>
       </c>
       <c r="F66">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G66">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="H66">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I66">
         <v>4</v>
       </c>
       <c r="J66">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K66">
+        <v>33</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>9</v>
+      </c>
+      <c r="N66">
+        <v>4</v>
+      </c>
+      <c r="O66">
+        <v>4</v>
+      </c>
+      <c r="P66">
+        <v>7</v>
+      </c>
+      <c r="Q66">
+        <v>10</v>
+      </c>
+      <c r="R66">
+        <v>15</v>
+      </c>
+      <c r="S66">
+        <v>4</v>
+      </c>
+      <c r="T66">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>43481</v>
+      </c>
+      <c r="B67" t="s">
+        <v>234</v>
+      </c>
+      <c r="D67">
+        <v>12</v>
+      </c>
+      <c r="E67">
+        <v>5</v>
+      </c>
+      <c r="F67">
+        <v>7</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="H67">
+        <v>6</v>
+      </c>
+      <c r="I67">
+        <v>6</v>
+      </c>
+      <c r="J67">
+        <v>4</v>
+      </c>
+      <c r="K67">
+        <v>31</v>
+      </c>
+      <c r="M67">
+        <v>7</v>
+      </c>
+      <c r="N67">
+        <v>4</v>
+      </c>
+      <c r="O67">
+        <v>5</v>
+      </c>
+      <c r="P67">
+        <v>6</v>
+      </c>
+      <c r="Q67">
+        <v>12</v>
+      </c>
+      <c r="R67">
+        <v>10</v>
+      </c>
+      <c r="S67">
+        <v>4</v>
+      </c>
+      <c r="T67">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>43481</v>
+      </c>
+      <c r="B68" t="s">
+        <v>235</v>
+      </c>
+      <c r="C68">
+        <v>6</v>
+      </c>
+      <c r="D68">
+        <v>6</v>
+      </c>
+      <c r="E68">
+        <v>5</v>
+      </c>
+      <c r="F68">
+        <v>9</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="H68">
+        <v>4</v>
+      </c>
+      <c r="I68">
+        <v>4</v>
+      </c>
+      <c r="J68">
+        <v>6</v>
+      </c>
+      <c r="K68">
         <v>32</v>
       </c>
-      <c r="L66">
-        <v>0</v>
-      </c>
-      <c r="M66">
-        <v>8</v>
-      </c>
-      <c r="N66">
-        <v>0</v>
-      </c>
-      <c r="O66">
-        <v>6</v>
-      </c>
-      <c r="P66">
-        <v>7</v>
-      </c>
-      <c r="Q66">
-        <v>6</v>
-      </c>
-      <c r="R66">
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>8</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>6</v>
+      </c>
+      <c r="P68">
+        <v>7</v>
+      </c>
+      <c r="Q68">
+        <v>6</v>
+      </c>
+      <c r="R68">
         <v>14</v>
       </c>
-      <c r="S66">
-        <v>0</v>
-      </c>
-      <c r="T66">
+      <c r="S68">
+        <v>0</v>
+      </c>
+      <c r="T68">
         <v>13</v>
       </c>
-      <c r="U66">
+      <c r="U68">
         <v>6</v>
       </c>
     </row>

</xml_diff>